<commit_message>
updates rxns and files
</commit_message>
<xml_diff>
--- a/ATLASX IDs_Saccharomyces.xlsx
+++ b/ATLASX IDs_Saccharomyces.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Procesamiento DB" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,7 +28,18 @@
   </authors>
   <commentList>
     <comment ref="D11" authorId="0">
-      <text/>
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+      </text>
     </comment>
     <comment ref="D12" authorId="0">
       <text>
@@ -69,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="142">
   <si>
     <t xml:space="preserve">I.D.</t>
   </si>
@@ -456,7 +467,7 @@
     <t xml:space="preserve">Ninguno.</t>
   </si>
   <si>
-    <t xml:space="preserve">added_34dhbz_34dhbzal</t>
+    <t xml:space="preserve">added_34dhbz_34dhbald</t>
   </si>
   <si>
     <t xml:space="preserve">car</t>
@@ -480,7 +491,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">34dhbzal_c</t>
+      <t xml:space="preserve">34dhbald_c</t>
     </r>
     <r>
       <rPr>
@@ -682,7 +693,7 @@
     <t xml:space="preserve">bmp12 no pudo ser expresada en E. coli ni porque le hayan optimizado codones… pero pobA sí.</t>
   </si>
   <si>
-    <t xml:space="preserve">added_4hbz_4hbzal</t>
+    <t xml:space="preserve">added_4hbz_4hbald</t>
   </si>
   <si>
     <r>
@@ -703,7 +714,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">4hbzal_c</t>
+      <t xml:space="preserve">4hbald_c</t>
     </r>
     <r>
       <rPr>
@@ -717,7 +728,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">added_4hbzal_34dhbzal</t>
+    <t xml:space="preserve">added_4hbald_34dhbald</t>
   </si>
   <si>
     <r>
@@ -753,7 +764,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">4hbzal_c + nadph_c + o2_c + h_c -&gt; </t>
+      <t xml:space="preserve">4hbald_c + nadph_c + o2_c + h_c -&gt; </t>
     </r>
     <r>
       <rPr>
@@ -763,7 +774,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">34dhbzal_c</t>
+      <t xml:space="preserve">34dhbald_c</t>
     </r>
     <r>
       <rPr>
@@ -888,7 +899,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">added_T4hcinnm_4hbzal</t>
+    <t xml:space="preserve">added_T4hcinnm_4hbald</t>
   </si>
   <si>
     <r>
@@ -934,7 +945,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> 4hbzal_c </t>
+      <t xml:space="preserve"> 4hbald_c </t>
     </r>
     <r>
       <rPr>
@@ -1209,6 +1220,38 @@
   </si>
   <si>
     <t xml:space="preserve">added_coucoa_caffcoa</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">coucoa_c + ??? → </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">caffcoa_c</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> + ???</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">added_coucoa_4hbald</t>
@@ -1365,7 +1408,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1481,6 +1524,12 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="12">
     <fill>
@@ -1550,7 +1599,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="30">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -1742,13 +1791,6 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left style="medium"/>
-      <right/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
       <right style="medium"/>
       <top style="thin"/>
       <bottom/>
@@ -1794,7 +1836,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="116">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2007,6 +2049,10 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2119,39 +2165,39 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="8" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="14" fillId="8" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2179,7 +2225,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="10" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="10" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2199,7 +2245,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="9" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="9" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2219,7 +2265,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="11" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="11" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2756,10 +2802,10 @@
   </sheetPr>
   <dimension ref="A2:G20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
+      <selection pane="bottomLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2813,7 +2859,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="114.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="91.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="44" t="s">
         <v>50</v>
       </c>
@@ -2873,7 +2919,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="114.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="91.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="44" t="s">
         <v>67</v>
       </c>
@@ -2893,7 +2939,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="57" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="44" t="s">
         <v>69</v>
       </c>
@@ -2933,7 +2979,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="35.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="44" t="s">
         <v>80</v>
       </c>
@@ -3058,24 +3104,26 @@
       <c r="F18" s="46"/>
       <c r="G18" s="46"/>
     </row>
-    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="52"/>
       <c r="B19" s="44" t="s">
         <v>101</v>
       </c>
       <c r="C19" s="45"/>
-      <c r="D19" s="46"/>
+      <c r="D19" s="46" t="s">
+        <v>102</v>
+      </c>
       <c r="E19" s="46"/>
       <c r="F19" s="46"/>
       <c r="G19" s="46"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="44" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C20" s="45"/>
       <c r="D20" s="46" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E20" s="46"/>
       <c r="F20" s="46"/>
@@ -3100,1213 +3148,1233 @@
   </sheetPr>
   <dimension ref="B1:Q46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M7" activeCellId="0" sqref="M7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="3" style="0" width="6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="53" width="3.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="53" width="31.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="3" style="53" width="6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="2" s="53" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="54" t="s">
-        <v>104</v>
-      </c>
-      <c r="C2" s="55" t="s">
+    <row r="2" s="54" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="55" t="s">
         <v>105</v>
       </c>
-      <c r="D2" s="56" t="s">
+      <c r="C2" s="56" t="s">
         <v>106</v>
       </c>
-      <c r="E2" s="57" t="s">
+      <c r="D2" s="57" t="s">
         <v>107</v>
       </c>
-      <c r="F2" s="56" t="s">
+      <c r="E2" s="58" t="s">
         <v>108</v>
       </c>
-      <c r="G2" s="58" t="s">
+      <c r="F2" s="57" t="s">
         <v>109</v>
       </c>
-      <c r="H2" s="59" t="s">
+      <c r="G2" s="59" t="s">
         <v>110</v>
       </c>
-      <c r="I2" s="60" t="s">
+      <c r="H2" s="60" t="s">
         <v>111</v>
       </c>
-      <c r="J2" s="58" t="s">
+      <c r="I2" s="61" t="s">
         <v>112</v>
       </c>
-      <c r="K2" s="58" t="s">
+      <c r="J2" s="59" t="s">
         <v>113</v>
       </c>
-      <c r="L2" s="58" t="s">
+      <c r="K2" s="59" t="s">
         <v>114</v>
       </c>
-      <c r="M2" s="58" t="s">
+      <c r="L2" s="59" t="s">
         <v>115</v>
       </c>
-      <c r="N2" s="58" t="s">
+      <c r="M2" s="59" t="s">
         <v>116</v>
       </c>
-      <c r="O2" s="61" t="s">
+      <c r="N2" s="59" t="s">
         <v>117</v>
       </c>
-      <c r="P2" s="61" t="s">
+      <c r="O2" s="62" t="s">
         <v>118</v>
       </c>
-      <c r="Q2" s="59" t="s">
+      <c r="P2" s="62" t="s">
         <v>119</v>
       </c>
+      <c r="Q2" s="60" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="62" t="s">
+      <c r="B3" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="63"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="68"/>
-      <c r="J3" s="66"/>
-      <c r="K3" s="66"/>
-      <c r="L3" s="66"/>
-      <c r="M3" s="66"/>
-      <c r="N3" s="66"/>
-      <c r="O3" s="69"/>
-      <c r="P3" s="69"/>
-      <c r="Q3" s="67"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="68"/>
+      <c r="I3" s="69"/>
+      <c r="J3" s="67"/>
+      <c r="K3" s="67"/>
+      <c r="L3" s="67"/>
+      <c r="M3" s="67"/>
+      <c r="N3" s="67"/>
+      <c r="O3" s="70"/>
+      <c r="P3" s="70"/>
+      <c r="Q3" s="68"/>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="62" t="s">
+      <c r="B4" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="63"/>
-      <c r="D4" s="70"/>
-      <c r="E4" s="65"/>
-      <c r="F4" s="64"/>
-      <c r="G4" s="66"/>
-      <c r="H4" s="67"/>
-      <c r="I4" s="68"/>
-      <c r="J4" s="66"/>
-      <c r="K4" s="66"/>
-      <c r="L4" s="66"/>
-      <c r="M4" s="66"/>
-      <c r="N4" s="66"/>
-      <c r="O4" s="69"/>
-      <c r="P4" s="69"/>
-      <c r="Q4" s="67"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="71"/>
+      <c r="E4" s="66"/>
+      <c r="F4" s="65"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="68"/>
+      <c r="I4" s="69"/>
+      <c r="J4" s="67"/>
+      <c r="K4" s="67"/>
+      <c r="L4" s="67"/>
+      <c r="M4" s="67"/>
+      <c r="N4" s="67"/>
+      <c r="O4" s="70"/>
+      <c r="P4" s="70"/>
+      <c r="Q4" s="68"/>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="62" t="s">
+      <c r="B5" s="63" t="s">
         <v>56</v>
       </c>
-      <c r="C5" s="71"/>
-      <c r="D5" s="72"/>
-      <c r="E5" s="73"/>
-      <c r="F5" s="72"/>
-      <c r="G5" s="74"/>
-      <c r="H5" s="67"/>
-      <c r="I5" s="75"/>
-      <c r="J5" s="74"/>
-      <c r="K5" s="74"/>
-      <c r="L5" s="74"/>
-      <c r="M5" s="74"/>
-      <c r="N5" s="74"/>
-      <c r="O5" s="69"/>
-      <c r="P5" s="69"/>
-      <c r="Q5" s="67"/>
+      <c r="C5" s="72"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="75"/>
+      <c r="H5" s="68"/>
+      <c r="I5" s="76"/>
+      <c r="J5" s="75"/>
+      <c r="K5" s="75"/>
+      <c r="L5" s="75"/>
+      <c r="M5" s="75"/>
+      <c r="N5" s="75"/>
+      <c r="O5" s="70"/>
+      <c r="P5" s="70"/>
+      <c r="Q5" s="68"/>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="76" t="s">
+      <c r="B6" s="77" t="s">
         <v>62</v>
       </c>
-      <c r="C6" s="77"/>
-      <c r="D6" s="70"/>
-      <c r="E6" s="65"/>
-      <c r="F6" s="64"/>
-      <c r="G6" s="66"/>
-      <c r="H6" s="67"/>
-      <c r="I6" s="68"/>
-      <c r="J6" s="66"/>
-      <c r="K6" s="66"/>
-      <c r="L6" s="66"/>
-      <c r="M6" s="66"/>
-      <c r="N6" s="66"/>
-      <c r="O6" s="69"/>
-      <c r="P6" s="69"/>
-      <c r="Q6" s="67"/>
+      <c r="C6" s="78"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="65"/>
+      <c r="G6" s="67"/>
+      <c r="H6" s="68"/>
+      <c r="I6" s="69"/>
+      <c r="J6" s="67"/>
+      <c r="K6" s="67"/>
+      <c r="L6" s="67"/>
+      <c r="M6" s="67"/>
+      <c r="N6" s="67"/>
+      <c r="O6" s="70"/>
+      <c r="P6" s="70"/>
+      <c r="Q6" s="68"/>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="76" t="s">
+      <c r="B7" s="77" t="s">
         <v>67</v>
       </c>
-      <c r="C7" s="77"/>
-      <c r="D7" s="64"/>
-      <c r="E7" s="78"/>
-      <c r="F7" s="64"/>
-      <c r="G7" s="66"/>
-      <c r="H7" s="67"/>
-      <c r="I7" s="68"/>
-      <c r="J7" s="66"/>
-      <c r="K7" s="66"/>
-      <c r="L7" s="66"/>
-      <c r="M7" s="66"/>
-      <c r="N7" s="66"/>
-      <c r="O7" s="69"/>
-      <c r="P7" s="69"/>
-      <c r="Q7" s="67"/>
+      <c r="C7" s="78"/>
+      <c r="D7" s="65"/>
+      <c r="E7" s="79"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="67"/>
+      <c r="H7" s="68"/>
+      <c r="I7" s="69"/>
+      <c r="J7" s="67"/>
+      <c r="K7" s="67"/>
+      <c r="L7" s="67"/>
+      <c r="M7" s="67"/>
+      <c r="N7" s="67"/>
+      <c r="O7" s="70"/>
+      <c r="P7" s="70"/>
+      <c r="Q7" s="68"/>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="76" t="s">
+      <c r="B8" s="77" t="s">
         <v>69</v>
       </c>
-      <c r="C8" s="77"/>
-      <c r="D8" s="64"/>
-      <c r="E8" s="78"/>
-      <c r="F8" s="70"/>
-      <c r="G8" s="79"/>
-      <c r="H8" s="67"/>
-      <c r="I8" s="68"/>
-      <c r="J8" s="66"/>
-      <c r="K8" s="66"/>
-      <c r="L8" s="66"/>
-      <c r="M8" s="66"/>
-      <c r="N8" s="66"/>
-      <c r="O8" s="69"/>
-      <c r="P8" s="69"/>
-      <c r="Q8" s="67"/>
+      <c r="C8" s="78"/>
+      <c r="D8" s="65"/>
+      <c r="E8" s="79"/>
+      <c r="F8" s="71"/>
+      <c r="G8" s="80"/>
+      <c r="H8" s="68"/>
+      <c r="I8" s="69"/>
+      <c r="J8" s="67"/>
+      <c r="K8" s="67"/>
+      <c r="L8" s="67"/>
+      <c r="M8" s="67"/>
+      <c r="N8" s="67"/>
+      <c r="O8" s="70"/>
+      <c r="P8" s="70"/>
+      <c r="Q8" s="68"/>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="76" t="s">
+      <c r="B9" s="77" t="s">
         <v>74</v>
       </c>
-      <c r="C9" s="77"/>
-      <c r="D9" s="64"/>
-      <c r="E9" s="65"/>
-      <c r="F9" s="70"/>
-      <c r="G9" s="79"/>
-      <c r="H9" s="67"/>
-      <c r="I9" s="68"/>
-      <c r="J9" s="66"/>
-      <c r="K9" s="66"/>
-      <c r="L9" s="66"/>
-      <c r="M9" s="66"/>
-      <c r="N9" s="66"/>
-      <c r="O9" s="69"/>
-      <c r="P9" s="69"/>
-      <c r="Q9" s="67"/>
+      <c r="C9" s="78"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="66"/>
+      <c r="F9" s="71"/>
+      <c r="G9" s="80"/>
+      <c r="H9" s="68"/>
+      <c r="I9" s="69"/>
+      <c r="J9" s="67"/>
+      <c r="K9" s="67"/>
+      <c r="L9" s="67"/>
+      <c r="M9" s="67"/>
+      <c r="N9" s="67"/>
+      <c r="O9" s="70"/>
+      <c r="P9" s="70"/>
+      <c r="Q9" s="68"/>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="76" t="s">
+      <c r="B10" s="77" t="s">
         <v>80</v>
       </c>
-      <c r="C10" s="77"/>
-      <c r="D10" s="64"/>
-      <c r="E10" s="65"/>
-      <c r="F10" s="70"/>
-      <c r="G10" s="79"/>
-      <c r="H10" s="67"/>
-      <c r="I10" s="68"/>
-      <c r="J10" s="66"/>
-      <c r="K10" s="66"/>
-      <c r="L10" s="66"/>
-      <c r="M10" s="66"/>
-      <c r="N10" s="66"/>
-      <c r="O10" s="69"/>
-      <c r="P10" s="69"/>
-      <c r="Q10" s="67"/>
+      <c r="C10" s="78"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="66"/>
+      <c r="F10" s="71"/>
+      <c r="G10" s="80"/>
+      <c r="H10" s="68"/>
+      <c r="I10" s="69"/>
+      <c r="J10" s="67"/>
+      <c r="K10" s="67"/>
+      <c r="L10" s="67"/>
+      <c r="M10" s="67"/>
+      <c r="N10" s="67"/>
+      <c r="O10" s="70"/>
+      <c r="P10" s="70"/>
+      <c r="Q10" s="68"/>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="76" t="s">
+      <c r="B11" s="77" t="s">
         <v>83</v>
       </c>
-      <c r="C11" s="77"/>
-      <c r="D11" s="64"/>
-      <c r="E11" s="65"/>
-      <c r="F11" s="64"/>
-      <c r="G11" s="80"/>
-      <c r="H11" s="67"/>
-      <c r="I11" s="68"/>
-      <c r="J11" s="66"/>
-      <c r="K11" s="66"/>
-      <c r="L11" s="80"/>
-      <c r="M11" s="80"/>
-      <c r="N11" s="80"/>
-      <c r="O11" s="69"/>
-      <c r="P11" s="69"/>
-      <c r="Q11" s="67"/>
+      <c r="C11" s="78"/>
+      <c r="D11" s="65"/>
+      <c r="E11" s="66"/>
+      <c r="F11" s="65"/>
+      <c r="G11" s="81"/>
+      <c r="H11" s="68"/>
+      <c r="I11" s="69"/>
+      <c r="J11" s="67"/>
+      <c r="K11" s="67"/>
+      <c r="L11" s="81"/>
+      <c r="M11" s="81"/>
+      <c r="N11" s="81"/>
+      <c r="O11" s="70"/>
+      <c r="P11" s="70"/>
+      <c r="Q11" s="68"/>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="76" t="s">
+      <c r="B12" s="77" t="s">
         <v>86</v>
       </c>
-      <c r="C12" s="77"/>
-      <c r="D12" s="64"/>
-      <c r="E12" s="65"/>
-      <c r="F12" s="64"/>
-      <c r="G12" s="80"/>
-      <c r="H12" s="67"/>
-      <c r="I12" s="68"/>
-      <c r="J12" s="66"/>
-      <c r="K12" s="66"/>
-      <c r="L12" s="80"/>
-      <c r="M12" s="80"/>
-      <c r="N12" s="80"/>
-      <c r="O12" s="69"/>
-      <c r="P12" s="69"/>
-      <c r="Q12" s="67"/>
+      <c r="C12" s="78"/>
+      <c r="D12" s="65"/>
+      <c r="E12" s="66"/>
+      <c r="F12" s="65"/>
+      <c r="G12" s="81"/>
+      <c r="H12" s="68"/>
+      <c r="I12" s="69"/>
+      <c r="J12" s="67"/>
+      <c r="K12" s="67"/>
+      <c r="L12" s="81"/>
+      <c r="M12" s="81"/>
+      <c r="N12" s="81"/>
+      <c r="O12" s="70"/>
+      <c r="P12" s="70"/>
+      <c r="Q12" s="68"/>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="76" t="s">
+      <c r="B13" s="77" t="s">
         <v>92</v>
       </c>
-      <c r="C13" s="77"/>
-      <c r="D13" s="64"/>
-      <c r="E13" s="65"/>
-      <c r="F13" s="64"/>
-      <c r="G13" s="66"/>
-      <c r="H13" s="67"/>
-      <c r="I13" s="68"/>
-      <c r="J13" s="66"/>
-      <c r="K13" s="66"/>
-      <c r="L13" s="66"/>
-      <c r="M13" s="66"/>
-      <c r="N13" s="66"/>
-      <c r="O13" s="69"/>
-      <c r="P13" s="69"/>
-      <c r="Q13" s="67"/>
-    </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="76"/>
-      <c r="C14" s="77"/>
-      <c r="D14" s="64"/>
-      <c r="E14" s="65"/>
-      <c r="F14" s="64"/>
-      <c r="G14" s="66"/>
-      <c r="H14" s="67"/>
-      <c r="I14" s="68"/>
-      <c r="J14" s="66"/>
-      <c r="K14" s="66"/>
-      <c r="L14" s="66"/>
-      <c r="M14" s="66"/>
-      <c r="N14" s="66"/>
-      <c r="O14" s="69"/>
-      <c r="P14" s="69"/>
-    </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="76"/>
-      <c r="C15" s="77"/>
-      <c r="D15" s="64"/>
-      <c r="E15" s="65"/>
-      <c r="F15" s="64"/>
-      <c r="G15" s="66"/>
-      <c r="H15" s="67"/>
-      <c r="I15" s="68"/>
-      <c r="J15" s="66"/>
-      <c r="K15" s="66"/>
-      <c r="L15" s="66"/>
-      <c r="M15" s="66"/>
-      <c r="N15" s="66"/>
-      <c r="O15" s="69"/>
-      <c r="P15" s="69"/>
-    </row>
-    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="76"/>
-      <c r="C16" s="77"/>
-      <c r="D16" s="64"/>
-      <c r="E16" s="65"/>
-      <c r="F16" s="64"/>
-      <c r="G16" s="66"/>
-      <c r="H16" s="67"/>
-      <c r="I16" s="68"/>
-      <c r="J16" s="66"/>
-      <c r="K16" s="66"/>
-      <c r="L16" s="66"/>
-      <c r="M16" s="66"/>
-      <c r="N16" s="66"/>
-      <c r="O16" s="69"/>
-      <c r="P16" s="69"/>
-    </row>
-    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="76"/>
-      <c r="C17" s="77"/>
-      <c r="D17" s="64"/>
-      <c r="E17" s="65"/>
-      <c r="F17" s="64"/>
-      <c r="G17" s="66"/>
-      <c r="H17" s="67"/>
-      <c r="I17" s="68"/>
-      <c r="J17" s="66"/>
-      <c r="K17" s="66"/>
-      <c r="L17" s="66"/>
-      <c r="M17" s="66"/>
-      <c r="N17" s="66"/>
-      <c r="O17" s="69"/>
-      <c r="P17" s="69"/>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="81"/>
-      <c r="C18" s="82"/>
-      <c r="D18" s="83"/>
-      <c r="E18" s="84"/>
-      <c r="F18" s="83"/>
-      <c r="G18" s="85"/>
-      <c r="H18" s="86"/>
-      <c r="I18" s="87"/>
-      <c r="J18" s="85"/>
-      <c r="K18" s="85"/>
-      <c r="L18" s="85"/>
-      <c r="M18" s="85"/>
-      <c r="N18" s="85"/>
-      <c r="O18" s="88"/>
-      <c r="P18" s="88"/>
+      <c r="C13" s="78"/>
+      <c r="D13" s="65"/>
+      <c r="E13" s="66"/>
+      <c r="F13" s="65"/>
+      <c r="G13" s="67"/>
+      <c r="H13" s="68"/>
+      <c r="I13" s="69"/>
+      <c r="J13" s="67"/>
+      <c r="K13" s="67"/>
+      <c r="L13" s="67"/>
+      <c r="M13" s="67"/>
+      <c r="N13" s="67"/>
+      <c r="O13" s="70"/>
+      <c r="P13" s="70"/>
+      <c r="Q13" s="68"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="82" t="s">
+        <v>95</v>
+      </c>
+      <c r="C14" s="78"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="66"/>
+      <c r="F14" s="65"/>
+      <c r="G14" s="67"/>
+      <c r="H14" s="68"/>
+      <c r="I14" s="69"/>
+      <c r="J14" s="67"/>
+      <c r="K14" s="67"/>
+      <c r="L14" s="67"/>
+      <c r="M14" s="67"/>
+      <c r="N14" s="67"/>
+      <c r="O14" s="70"/>
+      <c r="P14" s="70"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="82" t="s">
+        <v>97</v>
+      </c>
+      <c r="C15" s="78"/>
+      <c r="D15" s="65"/>
+      <c r="E15" s="66"/>
+      <c r="F15" s="65"/>
+      <c r="G15" s="67"/>
+      <c r="H15" s="68"/>
+      <c r="I15" s="69"/>
+      <c r="J15" s="67"/>
+      <c r="K15" s="67"/>
+      <c r="L15" s="67"/>
+      <c r="M15" s="67"/>
+      <c r="N15" s="67"/>
+      <c r="O15" s="70"/>
+      <c r="P15" s="70"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="82" t="s">
+        <v>99</v>
+      </c>
+      <c r="C16" s="78"/>
+      <c r="D16" s="65"/>
+      <c r="E16" s="66"/>
+      <c r="F16" s="65"/>
+      <c r="G16" s="67"/>
+      <c r="H16" s="68"/>
+      <c r="I16" s="69"/>
+      <c r="J16" s="67"/>
+      <c r="K16" s="67"/>
+      <c r="L16" s="67"/>
+      <c r="M16" s="67"/>
+      <c r="N16" s="67"/>
+      <c r="O16" s="70"/>
+      <c r="P16" s="70"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="82" t="s">
+        <v>101</v>
+      </c>
+      <c r="C17" s="78"/>
+      <c r="D17" s="65"/>
+      <c r="E17" s="66"/>
+      <c r="F17" s="65"/>
+      <c r="G17" s="67"/>
+      <c r="H17" s="68"/>
+      <c r="I17" s="69"/>
+      <c r="J17" s="67"/>
+      <c r="K17" s="67"/>
+      <c r="L17" s="67"/>
+      <c r="M17" s="67"/>
+      <c r="N17" s="67"/>
+      <c r="O17" s="70"/>
+      <c r="P17" s="70"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="82" t="s">
+        <v>103</v>
+      </c>
+      <c r="C18" s="83"/>
+      <c r="D18" s="84"/>
+      <c r="E18" s="85"/>
+      <c r="F18" s="84"/>
+      <c r="G18" s="86"/>
+      <c r="H18" s="87"/>
+      <c r="I18" s="88"/>
+      <c r="J18" s="86"/>
+      <c r="K18" s="86"/>
+      <c r="L18" s="86"/>
+      <c r="M18" s="86"/>
+      <c r="N18" s="86"/>
+      <c r="O18" s="89"/>
+      <c r="P18" s="89"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="89" t="s">
-        <v>120</v>
-      </c>
-      <c r="C19" s="90" t="n">
+      <c r="B19" s="90" t="s">
+        <v>121</v>
+      </c>
+      <c r="C19" s="91" t="n">
         <v>4</v>
       </c>
-      <c r="D19" s="91" t="n">
+      <c r="D19" s="92" t="n">
         <v>9</v>
       </c>
-      <c r="E19" s="92" t="n">
+      <c r="E19" s="93" t="n">
         <v>9</v>
       </c>
-      <c r="F19" s="91" t="n">
+      <c r="F19" s="92" t="n">
         <v>12</v>
       </c>
-      <c r="G19" s="93" t="n">
+      <c r="G19" s="94" t="n">
         <v>12</v>
       </c>
-      <c r="H19" s="94"/>
-      <c r="I19" s="91" t="n">
+      <c r="H19" s="95"/>
+      <c r="I19" s="92" t="n">
         <v>13</v>
       </c>
-      <c r="J19" s="93" t="n">
+      <c r="J19" s="94" t="n">
         <v>13</v>
       </c>
-      <c r="K19" s="93" t="n">
+      <c r="K19" s="94" t="n">
         <v>13</v>
       </c>
-      <c r="L19" s="93" t="n">
+      <c r="L19" s="94" t="n">
         <v>13</v>
       </c>
-      <c r="M19" s="93" t="n">
+      <c r="M19" s="94" t="n">
         <v>13</v>
       </c>
-      <c r="N19" s="93" t="n">
+      <c r="N19" s="94" t="n">
         <v>13</v>
       </c>
-      <c r="O19" s="95"/>
-      <c r="P19" s="95"/>
-      <c r="Q19" s="94"/>
+      <c r="O19" s="96"/>
+      <c r="P19" s="96"/>
+      <c r="Q19" s="95"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="89" t="s">
-        <v>121</v>
-      </c>
-      <c r="C20" s="90" t="n">
+      <c r="B20" s="90" t="s">
+        <v>122</v>
+      </c>
+      <c r="C20" s="91" t="n">
         <v>2</v>
       </c>
-      <c r="D20" s="91" t="n">
+      <c r="D20" s="92" t="n">
         <v>7</v>
       </c>
-      <c r="E20" s="92" t="n">
+      <c r="E20" s="93" t="n">
         <v>7</v>
       </c>
-      <c r="F20" s="91" t="n">
+      <c r="F20" s="92" t="n">
         <v>9</v>
       </c>
-      <c r="G20" s="93" t="n">
+      <c r="G20" s="94" t="n">
         <v>7</v>
       </c>
-      <c r="H20" s="94"/>
-      <c r="I20" s="91"/>
-      <c r="J20" s="93"/>
-      <c r="K20" s="93"/>
-      <c r="L20" s="93"/>
-      <c r="M20" s="93"/>
-      <c r="N20" s="93"/>
-      <c r="O20" s="95"/>
-      <c r="P20" s="95"/>
-      <c r="Q20" s="94"/>
+      <c r="H20" s="95"/>
+      <c r="I20" s="92"/>
+      <c r="J20" s="94"/>
+      <c r="K20" s="94"/>
+      <c r="L20" s="94"/>
+      <c r="M20" s="94"/>
+      <c r="N20" s="94"/>
+      <c r="O20" s="96"/>
+      <c r="P20" s="96"/>
+      <c r="Q20" s="95"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="96" t="s">
-        <v>122</v>
-      </c>
-      <c r="C21" s="97" t="n">
+      <c r="B21" s="97" t="s">
+        <v>123</v>
+      </c>
+      <c r="C21" s="98" t="n">
         <v>1</v>
       </c>
-      <c r="D21" s="98" t="n">
+      <c r="D21" s="99" t="n">
         <v>1</v>
       </c>
-      <c r="E21" s="99" t="n">
+      <c r="E21" s="100" t="n">
         <v>1</v>
       </c>
-      <c r="F21" s="98" t="n">
+      <c r="F21" s="99" t="n">
         <v>1</v>
       </c>
-      <c r="G21" s="100" t="n">
+      <c r="G21" s="101" t="n">
         <v>1</v>
       </c>
-      <c r="H21" s="94"/>
-      <c r="I21" s="98" t="n">
+      <c r="H21" s="95"/>
+      <c r="I21" s="99" t="n">
         <v>1</v>
       </c>
-      <c r="J21" s="100" t="n">
+      <c r="J21" s="101" t="n">
         <v>1</v>
       </c>
-      <c r="K21" s="100" t="n">
+      <c r="K21" s="101" t="n">
         <v>1</v>
       </c>
-      <c r="L21" s="100" t="n">
+      <c r="L21" s="101" t="n">
         <v>1</v>
       </c>
-      <c r="M21" s="100" t="n">
+      <c r="M21" s="101" t="n">
         <v>1</v>
       </c>
-      <c r="N21" s="100" t="n">
+      <c r="N21" s="101" t="n">
         <v>1</v>
       </c>
-      <c r="O21" s="95"/>
-      <c r="P21" s="95"/>
-      <c r="Q21" s="94"/>
+      <c r="O21" s="96"/>
+      <c r="P21" s="96"/>
+      <c r="Q21" s="95"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="101" t="s">
-        <v>123</v>
-      </c>
-      <c r="C22" s="102" t="n">
+      <c r="B22" s="102" t="s">
+        <v>124</v>
+      </c>
+      <c r="C22" s="103" t="n">
         <f aca="false">C19-C20</f>
         <v>2</v>
       </c>
-      <c r="D22" s="103" t="n">
+      <c r="D22" s="104" t="n">
         <f aca="false">D19-D20</f>
         <v>2</v>
       </c>
-      <c r="E22" s="104" t="n">
+      <c r="E22" s="105" t="n">
         <f aca="false">E19-E20</f>
         <v>2</v>
       </c>
-      <c r="F22" s="103" t="n">
+      <c r="F22" s="104" t="n">
         <f aca="false">F19-F20</f>
         <v>3</v>
       </c>
-      <c r="G22" s="105" t="n">
+      <c r="G22" s="106" t="n">
         <f aca="false">G19-G20</f>
         <v>5</v>
       </c>
-      <c r="H22" s="94" t="n">
+      <c r="H22" s="95" t="n">
         <f aca="false">H19-H20</f>
         <v>0</v>
       </c>
-      <c r="I22" s="103" t="n">
+      <c r="I22" s="104" t="n">
         <f aca="false">I19-I20</f>
         <v>13</v>
       </c>
-      <c r="J22" s="105" t="n">
+      <c r="J22" s="106" t="n">
         <f aca="false">J19-J20</f>
         <v>13</v>
       </c>
-      <c r="K22" s="105" t="n">
+      <c r="K22" s="106" t="n">
         <f aca="false">K19-K20</f>
         <v>13</v>
       </c>
-      <c r="L22" s="105" t="n">
+      <c r="L22" s="106" t="n">
         <f aca="false">L19-L20</f>
         <v>13</v>
       </c>
-      <c r="M22" s="105" t="n">
+      <c r="M22" s="106" t="n">
         <f aca="false">M19-M20</f>
         <v>13</v>
       </c>
-      <c r="N22" s="105" t="n">
+      <c r="N22" s="106" t="n">
         <f aca="false">N19-N20</f>
         <v>13</v>
       </c>
-      <c r="O22" s="95" t="n">
+      <c r="O22" s="96" t="n">
         <f aca="false">O19-O20</f>
         <v>0</v>
       </c>
-      <c r="P22" s="95" t="n">
+      <c r="P22" s="96" t="n">
         <f aca="false">P19-P20</f>
         <v>0</v>
       </c>
-      <c r="Q22" s="94" t="n">
+      <c r="Q22" s="95" t="n">
         <f aca="false">Q19-Q20</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="106" t="s">
-        <v>124</v>
-      </c>
-      <c r="C23" s="107" t="n">
+      <c r="B23" s="107" t="s">
+        <v>125</v>
+      </c>
+      <c r="C23" s="108" t="n">
         <f aca="false">C22+C21</f>
         <v>3</v>
       </c>
-      <c r="D23" s="108" t="n">
+      <c r="D23" s="109" t="n">
         <f aca="false">D22+D21</f>
         <v>3</v>
       </c>
-      <c r="E23" s="109" t="n">
+      <c r="E23" s="110" t="n">
         <f aca="false">E22+E21</f>
         <v>3</v>
       </c>
-      <c r="F23" s="108" t="n">
+      <c r="F23" s="109" t="n">
         <f aca="false">F22+F21</f>
         <v>4</v>
       </c>
-      <c r="G23" s="110" t="n">
+      <c r="G23" s="111" t="n">
         <f aca="false">G22+G21</f>
         <v>6</v>
       </c>
-      <c r="H23" s="94" t="n">
+      <c r="H23" s="95" t="n">
         <f aca="false">H22+H21</f>
         <v>0</v>
       </c>
-      <c r="I23" s="108" t="n">
+      <c r="I23" s="109" t="n">
         <f aca="false">I22+I21</f>
         <v>14</v>
       </c>
-      <c r="J23" s="110" t="n">
+      <c r="J23" s="111" t="n">
         <f aca="false">J22+J21</f>
         <v>14</v>
       </c>
-      <c r="K23" s="110" t="n">
+      <c r="K23" s="111" t="n">
         <f aca="false">K22+K21</f>
         <v>14</v>
       </c>
-      <c r="L23" s="110" t="n">
+      <c r="L23" s="111" t="n">
         <f aca="false">L22+L21</f>
         <v>14</v>
       </c>
-      <c r="M23" s="110" t="n">
+      <c r="M23" s="111" t="n">
         <f aca="false">M22+M21</f>
         <v>14</v>
       </c>
-      <c r="N23" s="110" t="n">
+      <c r="N23" s="111" t="n">
         <f aca="false">N22+N21</f>
         <v>14</v>
       </c>
-      <c r="O23" s="95" t="n">
+      <c r="O23" s="96" t="n">
         <f aca="false">O22+O21</f>
         <v>0</v>
       </c>
-      <c r="P23" s="95" t="n">
+      <c r="P23" s="96" t="n">
         <f aca="false">P22+P21</f>
         <v>0</v>
       </c>
-      <c r="Q23" s="94" t="n">
+      <c r="Q23" s="95" t="n">
         <f aca="false">Q22+Q21</f>
         <v>0</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="25" s="53" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="54" t="s">
-        <v>125</v>
-      </c>
-      <c r="C25" s="55" t="s">
+    <row r="25" s="54" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="55" t="s">
         <v>126</v>
       </c>
-      <c r="D25" s="56" t="s">
+      <c r="C25" s="56" t="s">
         <v>127</v>
       </c>
-      <c r="E25" s="57" t="s">
+      <c r="D25" s="57" t="s">
         <v>128</v>
       </c>
-      <c r="F25" s="56" t="s">
+      <c r="E25" s="58" t="s">
         <v>129</v>
       </c>
-      <c r="G25" s="58" t="s">
+      <c r="F25" s="57" t="s">
         <v>130</v>
       </c>
-      <c r="H25" s="59" t="s">
+      <c r="G25" s="59" t="s">
         <v>131</v>
       </c>
-      <c r="I25" s="60" t="s">
+      <c r="H25" s="60" t="s">
         <v>132</v>
       </c>
-      <c r="J25" s="58" t="s">
+      <c r="I25" s="61" t="s">
         <v>133</v>
       </c>
-      <c r="K25" s="58" t="s">
+      <c r="J25" s="59" t="s">
         <v>134</v>
       </c>
-      <c r="L25" s="58" t="s">
+      <c r="K25" s="59" t="s">
         <v>135</v>
       </c>
-      <c r="M25" s="58" t="s">
+      <c r="L25" s="59" t="s">
         <v>136</v>
       </c>
-      <c r="N25" s="58" t="s">
+      <c r="M25" s="59" t="s">
         <v>137</v>
       </c>
-      <c r="O25" s="61" t="s">
+      <c r="N25" s="59" t="s">
         <v>138</v>
       </c>
-      <c r="P25" s="61" t="s">
+      <c r="O25" s="62" t="s">
         <v>139</v>
       </c>
-      <c r="Q25" s="59" t="s">
+      <c r="P25" s="62" t="s">
         <v>140</v>
       </c>
+      <c r="Q25" s="60" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="62" t="s">
+      <c r="B26" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="C26" s="63"/>
-      <c r="D26" s="64"/>
-      <c r="E26" s="65"/>
-      <c r="F26" s="64"/>
-      <c r="G26" s="66"/>
-      <c r="H26" s="67"/>
-      <c r="I26" s="68"/>
-      <c r="J26" s="66"/>
-      <c r="K26" s="66"/>
-      <c r="L26" s="66"/>
-      <c r="M26" s="66"/>
-      <c r="N26" s="66"/>
-      <c r="O26" s="69"/>
-      <c r="P26" s="69"/>
-      <c r="Q26" s="67"/>
+      <c r="C26" s="64"/>
+      <c r="D26" s="65"/>
+      <c r="E26" s="66"/>
+      <c r="F26" s="65"/>
+      <c r="G26" s="67"/>
+      <c r="H26" s="68"/>
+      <c r="I26" s="69"/>
+      <c r="J26" s="67"/>
+      <c r="K26" s="67"/>
+      <c r="L26" s="67"/>
+      <c r="M26" s="67"/>
+      <c r="N26" s="67"/>
+      <c r="O26" s="70"/>
+      <c r="P26" s="70"/>
+      <c r="Q26" s="68"/>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="62" t="s">
+      <c r="B27" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="C27" s="63"/>
-      <c r="D27" s="70"/>
-      <c r="E27" s="65"/>
-      <c r="F27" s="64"/>
-      <c r="G27" s="66"/>
-      <c r="H27" s="67"/>
-      <c r="I27" s="68"/>
-      <c r="J27" s="66"/>
-      <c r="K27" s="66"/>
-      <c r="L27" s="66"/>
-      <c r="M27" s="66"/>
-      <c r="N27" s="66"/>
-      <c r="O27" s="69"/>
-      <c r="P27" s="69"/>
-      <c r="Q27" s="67"/>
+      <c r="C27" s="64"/>
+      <c r="D27" s="71"/>
+      <c r="E27" s="66"/>
+      <c r="F27" s="65"/>
+      <c r="G27" s="67"/>
+      <c r="H27" s="68"/>
+      <c r="I27" s="69"/>
+      <c r="J27" s="67"/>
+      <c r="K27" s="67"/>
+      <c r="L27" s="67"/>
+      <c r="M27" s="67"/>
+      <c r="N27" s="67"/>
+      <c r="O27" s="70"/>
+      <c r="P27" s="70"/>
+      <c r="Q27" s="68"/>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="62" t="s">
+      <c r="B28" s="63" t="s">
         <v>56</v>
       </c>
-      <c r="C28" s="71"/>
-      <c r="D28" s="72"/>
-      <c r="E28" s="73"/>
-      <c r="F28" s="72"/>
-      <c r="G28" s="74"/>
-      <c r="H28" s="67"/>
-      <c r="I28" s="75"/>
-      <c r="J28" s="74"/>
-      <c r="K28" s="74"/>
-      <c r="L28" s="74"/>
-      <c r="M28" s="74"/>
-      <c r="N28" s="74"/>
-      <c r="O28" s="69"/>
-      <c r="P28" s="69"/>
-      <c r="Q28" s="67"/>
+      <c r="C28" s="72"/>
+      <c r="D28" s="73"/>
+      <c r="E28" s="74"/>
+      <c r="F28" s="73"/>
+      <c r="G28" s="75"/>
+      <c r="H28" s="68"/>
+      <c r="I28" s="76"/>
+      <c r="J28" s="75"/>
+      <c r="K28" s="75"/>
+      <c r="L28" s="75"/>
+      <c r="M28" s="75"/>
+      <c r="N28" s="75"/>
+      <c r="O28" s="70"/>
+      <c r="P28" s="70"/>
+      <c r="Q28" s="68"/>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="76" t="s">
+      <c r="B29" s="77" t="s">
         <v>62</v>
       </c>
-      <c r="C29" s="77"/>
-      <c r="D29" s="70"/>
-      <c r="E29" s="65"/>
-      <c r="F29" s="64"/>
-      <c r="G29" s="66"/>
-      <c r="H29" s="67"/>
-      <c r="I29" s="68"/>
-      <c r="J29" s="66"/>
-      <c r="K29" s="66"/>
-      <c r="L29" s="66"/>
-      <c r="M29" s="66"/>
-      <c r="N29" s="66"/>
-      <c r="O29" s="69"/>
-      <c r="P29" s="69"/>
-      <c r="Q29" s="67"/>
+      <c r="C29" s="78"/>
+      <c r="D29" s="71"/>
+      <c r="E29" s="66"/>
+      <c r="F29" s="65"/>
+      <c r="G29" s="67"/>
+      <c r="H29" s="68"/>
+      <c r="I29" s="69"/>
+      <c r="J29" s="67"/>
+      <c r="K29" s="67"/>
+      <c r="L29" s="67"/>
+      <c r="M29" s="67"/>
+      <c r="N29" s="67"/>
+      <c r="O29" s="70"/>
+      <c r="P29" s="70"/>
+      <c r="Q29" s="68"/>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="76" t="s">
+      <c r="B30" s="77" t="s">
         <v>67</v>
       </c>
-      <c r="C30" s="77"/>
-      <c r="D30" s="64"/>
-      <c r="E30" s="78"/>
-      <c r="F30" s="64"/>
-      <c r="G30" s="66"/>
-      <c r="H30" s="67"/>
-      <c r="I30" s="68"/>
-      <c r="J30" s="66"/>
-      <c r="K30" s="66"/>
-      <c r="L30" s="66"/>
-      <c r="M30" s="66"/>
-      <c r="N30" s="66"/>
-      <c r="O30" s="69"/>
-      <c r="P30" s="69"/>
-      <c r="Q30" s="67"/>
+      <c r="C30" s="78"/>
+      <c r="D30" s="65"/>
+      <c r="E30" s="79"/>
+      <c r="F30" s="65"/>
+      <c r="G30" s="67"/>
+      <c r="H30" s="68"/>
+      <c r="I30" s="69"/>
+      <c r="J30" s="67"/>
+      <c r="K30" s="67"/>
+      <c r="L30" s="67"/>
+      <c r="M30" s="67"/>
+      <c r="N30" s="67"/>
+      <c r="O30" s="70"/>
+      <c r="P30" s="70"/>
+      <c r="Q30" s="68"/>
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="76" t="s">
+      <c r="B31" s="77" t="s">
         <v>69</v>
       </c>
-      <c r="C31" s="77"/>
-      <c r="D31" s="64"/>
-      <c r="E31" s="78"/>
-      <c r="F31" s="70"/>
-      <c r="G31" s="79"/>
-      <c r="H31" s="67"/>
-      <c r="I31" s="68"/>
-      <c r="J31" s="66"/>
-      <c r="K31" s="66"/>
-      <c r="L31" s="66"/>
-      <c r="M31" s="66"/>
-      <c r="N31" s="66"/>
-      <c r="O31" s="69"/>
-      <c r="P31" s="69"/>
-      <c r="Q31" s="67"/>
+      <c r="C31" s="78"/>
+      <c r="D31" s="65"/>
+      <c r="E31" s="79"/>
+      <c r="F31" s="71"/>
+      <c r="G31" s="80"/>
+      <c r="H31" s="68"/>
+      <c r="I31" s="69"/>
+      <c r="J31" s="67"/>
+      <c r="K31" s="67"/>
+      <c r="L31" s="67"/>
+      <c r="M31" s="67"/>
+      <c r="N31" s="67"/>
+      <c r="O31" s="70"/>
+      <c r="P31" s="70"/>
+      <c r="Q31" s="68"/>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="76" t="s">
+      <c r="B32" s="77" t="s">
         <v>74</v>
       </c>
-      <c r="C32" s="77"/>
-      <c r="D32" s="64"/>
-      <c r="E32" s="65"/>
-      <c r="F32" s="70"/>
-      <c r="G32" s="79"/>
-      <c r="H32" s="67"/>
-      <c r="I32" s="68"/>
-      <c r="J32" s="66"/>
-      <c r="K32" s="66"/>
-      <c r="L32" s="66"/>
-      <c r="M32" s="66"/>
-      <c r="N32" s="66"/>
-      <c r="O32" s="69"/>
-      <c r="P32" s="69"/>
-      <c r="Q32" s="67"/>
+      <c r="C32" s="78"/>
+      <c r="D32" s="65"/>
+      <c r="E32" s="66"/>
+      <c r="F32" s="71"/>
+      <c r="G32" s="80"/>
+      <c r="H32" s="68"/>
+      <c r="I32" s="69"/>
+      <c r="J32" s="67"/>
+      <c r="K32" s="67"/>
+      <c r="L32" s="67"/>
+      <c r="M32" s="67"/>
+      <c r="N32" s="67"/>
+      <c r="O32" s="70"/>
+      <c r="P32" s="70"/>
+      <c r="Q32" s="68"/>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="76" t="s">
+      <c r="B33" s="77" t="s">
         <v>80</v>
       </c>
-      <c r="C33" s="77"/>
-      <c r="D33" s="64"/>
-      <c r="E33" s="65"/>
-      <c r="F33" s="70"/>
-      <c r="G33" s="79"/>
-      <c r="H33" s="67"/>
-      <c r="I33" s="68"/>
-      <c r="J33" s="66"/>
-      <c r="K33" s="66"/>
-      <c r="L33" s="66"/>
-      <c r="M33" s="66"/>
-      <c r="N33" s="66"/>
-      <c r="O33" s="69"/>
-      <c r="P33" s="69"/>
-      <c r="Q33" s="67"/>
+      <c r="C33" s="78"/>
+      <c r="D33" s="65"/>
+      <c r="E33" s="66"/>
+      <c r="F33" s="71"/>
+      <c r="G33" s="80"/>
+      <c r="H33" s="68"/>
+      <c r="I33" s="69"/>
+      <c r="J33" s="67"/>
+      <c r="K33" s="67"/>
+      <c r="L33" s="67"/>
+      <c r="M33" s="67"/>
+      <c r="N33" s="67"/>
+      <c r="O33" s="70"/>
+      <c r="P33" s="70"/>
+      <c r="Q33" s="68"/>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="76" t="s">
+      <c r="B34" s="77" t="s">
         <v>83</v>
       </c>
-      <c r="C34" s="111"/>
-      <c r="D34" s="112"/>
-      <c r="E34" s="113"/>
-      <c r="F34" s="112"/>
-      <c r="G34" s="80"/>
-      <c r="H34" s="67"/>
-      <c r="I34" s="114"/>
-      <c r="J34" s="80"/>
-      <c r="K34" s="80"/>
-      <c r="L34" s="80"/>
-      <c r="M34" s="80"/>
-      <c r="N34" s="80"/>
-      <c r="O34" s="69"/>
-      <c r="P34" s="69"/>
-      <c r="Q34" s="67"/>
+      <c r="C34" s="112"/>
+      <c r="D34" s="113"/>
+      <c r="E34" s="114"/>
+      <c r="F34" s="113"/>
+      <c r="G34" s="81"/>
+      <c r="H34" s="68"/>
+      <c r="I34" s="115"/>
+      <c r="J34" s="81"/>
+      <c r="K34" s="81"/>
+      <c r="L34" s="81"/>
+      <c r="M34" s="81"/>
+      <c r="N34" s="81"/>
+      <c r="O34" s="70"/>
+      <c r="P34" s="70"/>
+      <c r="Q34" s="68"/>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="76" t="s">
+      <c r="B35" s="77" t="s">
         <v>86</v>
       </c>
-      <c r="C35" s="111"/>
-      <c r="D35" s="112"/>
-      <c r="E35" s="113"/>
-      <c r="F35" s="112"/>
-      <c r="G35" s="80"/>
-      <c r="H35" s="67"/>
-      <c r="I35" s="114"/>
-      <c r="J35" s="80"/>
-      <c r="K35" s="80"/>
-      <c r="L35" s="80"/>
-      <c r="M35" s="80"/>
-      <c r="N35" s="80"/>
-      <c r="O35" s="69"/>
-      <c r="P35" s="69"/>
-      <c r="Q35" s="67"/>
+      <c r="C35" s="112"/>
+      <c r="D35" s="113"/>
+      <c r="E35" s="114"/>
+      <c r="F35" s="113"/>
+      <c r="G35" s="81"/>
+      <c r="H35" s="68"/>
+      <c r="I35" s="115"/>
+      <c r="J35" s="81"/>
+      <c r="K35" s="81"/>
+      <c r="L35" s="81"/>
+      <c r="M35" s="81"/>
+      <c r="N35" s="81"/>
+      <c r="O35" s="70"/>
+      <c r="P35" s="70"/>
+      <c r="Q35" s="68"/>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="76" t="s">
+      <c r="B36" s="77" t="s">
         <v>92</v>
       </c>
-      <c r="C36" s="77"/>
-      <c r="D36" s="64"/>
-      <c r="E36" s="65"/>
-      <c r="F36" s="64"/>
-      <c r="G36" s="66"/>
-      <c r="H36" s="67"/>
-      <c r="I36" s="68"/>
-      <c r="J36" s="66"/>
-      <c r="K36" s="66"/>
-      <c r="L36" s="66"/>
-      <c r="M36" s="66"/>
-      <c r="N36" s="66"/>
-      <c r="O36" s="69"/>
-      <c r="P36" s="69"/>
-      <c r="Q36" s="67"/>
-    </row>
-    <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="76"/>
-      <c r="C37" s="77"/>
-      <c r="D37" s="64"/>
-      <c r="E37" s="65"/>
-      <c r="F37" s="64"/>
-      <c r="G37" s="66"/>
-      <c r="H37" s="67"/>
-      <c r="I37" s="68"/>
-      <c r="J37" s="66"/>
-      <c r="K37" s="66"/>
-      <c r="L37" s="66"/>
-      <c r="M37" s="66"/>
-      <c r="N37" s="66"/>
-      <c r="O37" s="69"/>
-      <c r="P37" s="69"/>
-    </row>
-    <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="76"/>
-      <c r="C38" s="77"/>
-      <c r="D38" s="64"/>
-      <c r="E38" s="65"/>
-      <c r="F38" s="64"/>
-      <c r="G38" s="66"/>
-      <c r="H38" s="67"/>
-      <c r="I38" s="68"/>
-      <c r="J38" s="66"/>
-      <c r="K38" s="66"/>
-      <c r="L38" s="66"/>
-      <c r="M38" s="66"/>
-      <c r="N38" s="66"/>
-      <c r="O38" s="69"/>
-      <c r="P38" s="69"/>
-    </row>
-    <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="76"/>
-      <c r="C39" s="77"/>
-      <c r="D39" s="64"/>
-      <c r="E39" s="65"/>
-      <c r="F39" s="64"/>
-      <c r="G39" s="66"/>
-      <c r="H39" s="67"/>
-      <c r="I39" s="68"/>
-      <c r="J39" s="66"/>
-      <c r="K39" s="66"/>
-      <c r="L39" s="66"/>
-      <c r="M39" s="66"/>
-      <c r="N39" s="66"/>
-      <c r="O39" s="69"/>
-      <c r="P39" s="69"/>
-    </row>
-    <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="76"/>
-      <c r="C40" s="77"/>
-      <c r="D40" s="64"/>
-      <c r="E40" s="65"/>
-      <c r="F40" s="64"/>
-      <c r="G40" s="66"/>
-      <c r="H40" s="67"/>
-      <c r="I40" s="68"/>
-      <c r="J40" s="66"/>
-      <c r="K40" s="66"/>
-      <c r="L40" s="66"/>
-      <c r="M40" s="66"/>
-      <c r="N40" s="66"/>
-      <c r="O40" s="69"/>
-      <c r="P40" s="69"/>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="81"/>
-      <c r="C41" s="82"/>
-      <c r="D41" s="83"/>
-      <c r="E41" s="84"/>
-      <c r="F41" s="83"/>
-      <c r="G41" s="85"/>
-      <c r="H41" s="86"/>
-      <c r="I41" s="87"/>
-      <c r="J41" s="85"/>
-      <c r="K41" s="85"/>
-      <c r="L41" s="85"/>
-      <c r="M41" s="85"/>
-      <c r="N41" s="85"/>
-      <c r="O41" s="88"/>
-      <c r="P41" s="88"/>
+      <c r="C36" s="78"/>
+      <c r="D36" s="65"/>
+      <c r="E36" s="66"/>
+      <c r="F36" s="65"/>
+      <c r="G36" s="67"/>
+      <c r="H36" s="68"/>
+      <c r="I36" s="69"/>
+      <c r="J36" s="67"/>
+      <c r="K36" s="67"/>
+      <c r="L36" s="67"/>
+      <c r="M36" s="67"/>
+      <c r="N36" s="67"/>
+      <c r="O36" s="70"/>
+      <c r="P36" s="70"/>
+      <c r="Q36" s="68"/>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="82" t="s">
+        <v>95</v>
+      </c>
+      <c r="C37" s="78"/>
+      <c r="D37" s="65"/>
+      <c r="E37" s="66"/>
+      <c r="F37" s="65"/>
+      <c r="G37" s="67"/>
+      <c r="H37" s="68"/>
+      <c r="I37" s="69"/>
+      <c r="J37" s="67"/>
+      <c r="K37" s="67"/>
+      <c r="L37" s="67"/>
+      <c r="M37" s="67"/>
+      <c r="N37" s="67"/>
+      <c r="O37" s="70"/>
+      <c r="P37" s="70"/>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="82" t="s">
+        <v>97</v>
+      </c>
+      <c r="C38" s="78"/>
+      <c r="D38" s="65"/>
+      <c r="E38" s="66"/>
+      <c r="F38" s="65"/>
+      <c r="G38" s="67"/>
+      <c r="H38" s="68"/>
+      <c r="I38" s="69"/>
+      <c r="J38" s="67"/>
+      <c r="K38" s="67"/>
+      <c r="L38" s="67"/>
+      <c r="M38" s="67"/>
+      <c r="N38" s="67"/>
+      <c r="O38" s="70"/>
+      <c r="P38" s="70"/>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="82" t="s">
+        <v>99</v>
+      </c>
+      <c r="C39" s="78"/>
+      <c r="D39" s="65"/>
+      <c r="E39" s="66"/>
+      <c r="F39" s="65"/>
+      <c r="G39" s="67"/>
+      <c r="H39" s="68"/>
+      <c r="I39" s="69"/>
+      <c r="J39" s="67"/>
+      <c r="K39" s="67"/>
+      <c r="L39" s="67"/>
+      <c r="M39" s="67"/>
+      <c r="N39" s="67"/>
+      <c r="O39" s="70"/>
+      <c r="P39" s="70"/>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="82" t="s">
+        <v>101</v>
+      </c>
+      <c r="C40" s="78"/>
+      <c r="D40" s="65"/>
+      <c r="E40" s="66"/>
+      <c r="F40" s="65"/>
+      <c r="G40" s="67"/>
+      <c r="H40" s="68"/>
+      <c r="I40" s="69"/>
+      <c r="J40" s="67"/>
+      <c r="K40" s="67"/>
+      <c r="L40" s="67"/>
+      <c r="M40" s="67"/>
+      <c r="N40" s="67"/>
+      <c r="O40" s="70"/>
+      <c r="P40" s="70"/>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="82" t="s">
+        <v>103</v>
+      </c>
+      <c r="C41" s="83"/>
+      <c r="D41" s="84"/>
+      <c r="E41" s="85"/>
+      <c r="F41" s="84"/>
+      <c r="G41" s="86"/>
+      <c r="H41" s="87"/>
+      <c r="I41" s="88"/>
+      <c r="J41" s="86"/>
+      <c r="K41" s="86"/>
+      <c r="L41" s="86"/>
+      <c r="M41" s="86"/>
+      <c r="N41" s="86"/>
+      <c r="O41" s="89"/>
+      <c r="P41" s="89"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="89" t="s">
-        <v>120</v>
-      </c>
-      <c r="C42" s="90" t="n">
+      <c r="B42" s="90" t="s">
+        <v>121</v>
+      </c>
+      <c r="C42" s="91" t="n">
         <v>4</v>
       </c>
-      <c r="D42" s="91" t="n">
+      <c r="D42" s="92" t="n">
         <v>9</v>
       </c>
-      <c r="E42" s="92" t="n">
+      <c r="E42" s="93" t="n">
         <v>9</v>
       </c>
-      <c r="F42" s="91" t="n">
+      <c r="F42" s="92" t="n">
         <v>12</v>
       </c>
-      <c r="G42" s="93" t="n">
+      <c r="G42" s="94" t="n">
         <v>12</v>
       </c>
-      <c r="H42" s="94"/>
-      <c r="I42" s="91" t="n">
+      <c r="H42" s="95"/>
+      <c r="I42" s="92" t="n">
         <v>13</v>
       </c>
-      <c r="J42" s="93" t="n">
+      <c r="J42" s="94" t="n">
         <v>13</v>
       </c>
-      <c r="K42" s="93" t="n">
+      <c r="K42" s="94" t="n">
         <v>13</v>
       </c>
-      <c r="L42" s="93" t="n">
+      <c r="L42" s="94" t="n">
         <v>13</v>
       </c>
-      <c r="M42" s="93" t="n">
+      <c r="M42" s="94" t="n">
         <v>13</v>
       </c>
-      <c r="N42" s="93" t="n">
+      <c r="N42" s="94" t="n">
         <v>13</v>
       </c>
-      <c r="O42" s="95"/>
-      <c r="P42" s="95"/>
-      <c r="Q42" s="94"/>
+      <c r="O42" s="96"/>
+      <c r="P42" s="96"/>
+      <c r="Q42" s="95"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="89" t="s">
-        <v>121</v>
-      </c>
-      <c r="C43" s="90" t="n">
+      <c r="B43" s="90" t="s">
+        <v>122</v>
+      </c>
+      <c r="C43" s="91" t="n">
         <v>2</v>
       </c>
-      <c r="D43" s="91" t="n">
+      <c r="D43" s="92" t="n">
         <v>7</v>
       </c>
-      <c r="E43" s="92" t="n">
+      <c r="E43" s="93" t="n">
         <v>7</v>
       </c>
-      <c r="F43" s="91" t="n">
+      <c r="F43" s="92" t="n">
         <v>9</v>
       </c>
-      <c r="G43" s="93" t="n">
+      <c r="G43" s="94" t="n">
         <v>7</v>
       </c>
-      <c r="H43" s="94"/>
-      <c r="I43" s="91"/>
-      <c r="J43" s="93"/>
-      <c r="K43" s="93"/>
-      <c r="L43" s="93"/>
-      <c r="M43" s="93"/>
-      <c r="N43" s="93"/>
-      <c r="O43" s="95"/>
-      <c r="P43" s="95"/>
-      <c r="Q43" s="94"/>
+      <c r="H43" s="95"/>
+      <c r="I43" s="92"/>
+      <c r="J43" s="94"/>
+      <c r="K43" s="94"/>
+      <c r="L43" s="94"/>
+      <c r="M43" s="94"/>
+      <c r="N43" s="94"/>
+      <c r="O43" s="96"/>
+      <c r="P43" s="96"/>
+      <c r="Q43" s="95"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="96" t="s">
-        <v>122</v>
-      </c>
-      <c r="C44" s="97" t="n">
+      <c r="B44" s="97" t="s">
+        <v>123</v>
+      </c>
+      <c r="C44" s="98" t="n">
         <v>3</v>
       </c>
-      <c r="D44" s="98" t="n">
+      <c r="D44" s="99" t="n">
         <v>3</v>
       </c>
-      <c r="E44" s="99" t="n">
+      <c r="E44" s="100" t="n">
         <v>3</v>
       </c>
-      <c r="F44" s="98" t="n">
+      <c r="F44" s="99" t="n">
         <v>3</v>
       </c>
-      <c r="G44" s="100" t="n">
+      <c r="G44" s="101" t="n">
         <v>3</v>
       </c>
-      <c r="H44" s="94"/>
-      <c r="I44" s="98" t="n">
+      <c r="H44" s="95"/>
+      <c r="I44" s="99" t="n">
         <v>3</v>
       </c>
-      <c r="J44" s="100" t="n">
+      <c r="J44" s="101" t="n">
         <v>3</v>
       </c>
-      <c r="K44" s="100" t="n">
+      <c r="K44" s="101" t="n">
         <v>3</v>
       </c>
-      <c r="L44" s="100" t="n">
+      <c r="L44" s="101" t="n">
         <v>3</v>
       </c>
-      <c r="M44" s="100" t="n">
+      <c r="M44" s="101" t="n">
         <v>3</v>
       </c>
-      <c r="N44" s="100" t="n">
+      <c r="N44" s="101" t="n">
         <v>3</v>
       </c>
-      <c r="O44" s="95"/>
-      <c r="P44" s="95"/>
-      <c r="Q44" s="94"/>
+      <c r="O44" s="96"/>
+      <c r="P44" s="96"/>
+      <c r="Q44" s="95"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="101" t="s">
-        <v>123</v>
-      </c>
-      <c r="C45" s="102" t="n">
+      <c r="B45" s="102" t="s">
+        <v>124</v>
+      </c>
+      <c r="C45" s="103" t="n">
         <f aca="false">C42-C43</f>
         <v>2</v>
       </c>
-      <c r="D45" s="103" t="n">
+      <c r="D45" s="104" t="n">
         <f aca="false">D42-D43</f>
         <v>2</v>
       </c>
-      <c r="E45" s="104" t="n">
+      <c r="E45" s="105" t="n">
         <f aca="false">E42-E43</f>
         <v>2</v>
       </c>
-      <c r="F45" s="103" t="n">
+      <c r="F45" s="104" t="n">
         <f aca="false">F42-F43</f>
         <v>3</v>
       </c>
-      <c r="G45" s="105" t="n">
+      <c r="G45" s="106" t="n">
         <f aca="false">G42-G43</f>
         <v>5</v>
       </c>
-      <c r="H45" s="94" t="n">
+      <c r="H45" s="95" t="n">
         <f aca="false">H42-H43</f>
         <v>0</v>
       </c>
-      <c r="I45" s="103" t="n">
+      <c r="I45" s="104" t="n">
         <f aca="false">I42-I43</f>
         <v>13</v>
       </c>
-      <c r="J45" s="105" t="n">
+      <c r="J45" s="106" t="n">
         <f aca="false">J42-J43</f>
         <v>13</v>
       </c>
-      <c r="K45" s="105" t="n">
+      <c r="K45" s="106" t="n">
         <f aca="false">K42-K43</f>
         <v>13</v>
       </c>
-      <c r="L45" s="105" t="n">
+      <c r="L45" s="106" t="n">
         <f aca="false">L42-L43</f>
         <v>13</v>
       </c>
-      <c r="M45" s="105" t="n">
+      <c r="M45" s="106" t="n">
         <f aca="false">M42-M43</f>
         <v>13</v>
       </c>
-      <c r="N45" s="105" t="n">
+      <c r="N45" s="106" t="n">
         <f aca="false">N42-N43</f>
         <v>13</v>
       </c>
-      <c r="O45" s="95" t="n">
+      <c r="O45" s="96" t="n">
         <f aca="false">O42-O43</f>
         <v>0</v>
       </c>
-      <c r="P45" s="95" t="n">
+      <c r="P45" s="96" t="n">
         <f aca="false">P42-P43</f>
         <v>0</v>
       </c>
-      <c r="Q45" s="94" t="n">
+      <c r="Q45" s="95" t="n">
         <f aca="false">Q42-Q43</f>
         <v>0</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="106" t="s">
-        <v>124</v>
-      </c>
-      <c r="C46" s="107" t="n">
+      <c r="B46" s="107" t="s">
+        <v>125</v>
+      </c>
+      <c r="C46" s="108" t="n">
         <f aca="false">C45+C44</f>
         <v>5</v>
       </c>
-      <c r="D46" s="108" t="n">
+      <c r="D46" s="109" t="n">
         <f aca="false">D45+D44</f>
         <v>5</v>
       </c>
-      <c r="E46" s="109" t="n">
+      <c r="E46" s="110" t="n">
         <f aca="false">E45+E44</f>
         <v>5</v>
       </c>
-      <c r="F46" s="108" t="n">
+      <c r="F46" s="109" t="n">
         <f aca="false">F45+F44</f>
         <v>6</v>
       </c>
-      <c r="G46" s="110" t="n">
+      <c r="G46" s="111" t="n">
         <f aca="false">G45+G44</f>
         <v>8</v>
       </c>
-      <c r="H46" s="94" t="n">
+      <c r="H46" s="95" t="n">
         <f aca="false">H45+H44</f>
         <v>0</v>
       </c>
-      <c r="I46" s="108" t="n">
+      <c r="I46" s="109" t="n">
         <f aca="false">I45+I44</f>
         <v>16</v>
       </c>
-      <c r="J46" s="110" t="n">
+      <c r="J46" s="111" t="n">
         <f aca="false">J45+J44</f>
         <v>16</v>
       </c>
-      <c r="K46" s="110" t="n">
+      <c r="K46" s="111" t="n">
         <f aca="false">K45+K44</f>
         <v>16</v>
       </c>
-      <c r="L46" s="110" t="n">
+      <c r="L46" s="111" t="n">
         <f aca="false">L45+L44</f>
         <v>16</v>
       </c>
-      <c r="M46" s="110" t="n">
+      <c r="M46" s="111" t="n">
         <f aca="false">M45+M44</f>
         <v>16</v>
       </c>
-      <c r="N46" s="110" t="n">
+      <c r="N46" s="111" t="n">
         <f aca="false">N45+N44</f>
         <v>16</v>
       </c>
-      <c r="O46" s="95" t="n">
+      <c r="O46" s="96" t="n">
         <f aca="false">O45+O44</f>
         <v>0</v>
       </c>
-      <c r="P46" s="95" t="n">
+      <c r="P46" s="96" t="n">
         <f aca="false">P45+P44</f>
         <v>0</v>
       </c>
-      <c r="Q46" s="94" t="n">
+      <c r="Q46" s="95" t="n">
         <f aca="false">Q45+Q44</f>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
updated rxns after meeting
</commit_message>
<xml_diff>
--- a/ATLASX IDs_Saccharomyces.xlsx
+++ b/ATLASX IDs_Saccharomyces.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Procesamiento DB" sheetId="1" state="visible" r:id="rId2"/>
@@ -1230,7 +1230,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">coucoa_c + ??? → </t>
+      <t xml:space="preserve">coucoa_c + h2o_c → </t>
     </r>
     <r>
       <rPr>
@@ -1250,7 +1250,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> + ???</t>
+      <t xml:space="preserve"> + 2 h_c</t>
     </r>
   </si>
   <si>
@@ -1408,7 +1408,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1526,6 +1526,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFC9211E"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -1583,7 +1590,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FF993300"/>
+        <bgColor rgb="FFC9211E"/>
       </patternFill>
     </fill>
     <fill>
@@ -1836,7 +1843,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="121">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2161,14 +2168,30 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="26" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="9" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2190,6 +2213,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2364,7 +2391,7 @@
       <rgbColor rgb="FF00B050"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FFC9211E"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
@@ -2802,10 +2829,10 @@
   </sheetPr>
   <dimension ref="A2:G20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="2" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+      <selection pane="bottomLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3148,8 +3175,8 @@
   </sheetPr>
   <dimension ref="B1:Q46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N43" activeCellId="0" sqref="N43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3322,10 +3349,10 @@
       <c r="H8" s="68"/>
       <c r="I8" s="69"/>
       <c r="J8" s="67"/>
-      <c r="K8" s="67"/>
+      <c r="K8" s="80"/>
       <c r="L8" s="67"/>
       <c r="M8" s="67"/>
-      <c r="N8" s="67"/>
+      <c r="N8" s="80"/>
       <c r="O8" s="70"/>
       <c r="P8" s="70"/>
       <c r="Q8" s="68"/>
@@ -3340,12 +3367,12 @@
       <c r="F9" s="71"/>
       <c r="G9" s="80"/>
       <c r="H9" s="68"/>
-      <c r="I9" s="69"/>
-      <c r="J9" s="67"/>
-      <c r="K9" s="67"/>
-      <c r="L9" s="67"/>
-      <c r="M9" s="67"/>
-      <c r="N9" s="67"/>
+      <c r="I9" s="81"/>
+      <c r="J9" s="80"/>
+      <c r="K9" s="80"/>
+      <c r="L9" s="80"/>
+      <c r="M9" s="80"/>
+      <c r="N9" s="80"/>
       <c r="O9" s="70"/>
       <c r="P9" s="70"/>
       <c r="Q9" s="68"/>
@@ -3378,14 +3405,14 @@
       <c r="D11" s="65"/>
       <c r="E11" s="66"/>
       <c r="F11" s="65"/>
-      <c r="G11" s="81"/>
+      <c r="G11" s="82"/>
       <c r="H11" s="68"/>
       <c r="I11" s="69"/>
       <c r="J11" s="67"/>
       <c r="K11" s="67"/>
-      <c r="L11" s="81"/>
-      <c r="M11" s="81"/>
-      <c r="N11" s="81"/>
+      <c r="L11" s="82"/>
+      <c r="M11" s="82"/>
+      <c r="N11" s="82"/>
       <c r="O11" s="70"/>
       <c r="P11" s="70"/>
       <c r="Q11" s="68"/>
@@ -3398,14 +3425,14 @@
       <c r="D12" s="65"/>
       <c r="E12" s="66"/>
       <c r="F12" s="65"/>
-      <c r="G12" s="81"/>
+      <c r="G12" s="82"/>
       <c r="H12" s="68"/>
-      <c r="I12" s="69"/>
+      <c r="I12" s="83"/>
       <c r="J12" s="67"/>
       <c r="K12" s="67"/>
-      <c r="L12" s="81"/>
-      <c r="M12" s="81"/>
-      <c r="N12" s="81"/>
+      <c r="L12" s="82"/>
+      <c r="M12" s="82"/>
+      <c r="N12" s="82"/>
       <c r="O12" s="70"/>
       <c r="P12" s="70"/>
       <c r="Q12" s="68"/>
@@ -3420,10 +3447,10 @@
       <c r="F13" s="65"/>
       <c r="G13" s="67"/>
       <c r="H13" s="68"/>
-      <c r="I13" s="69"/>
+      <c r="I13" s="84"/>
       <c r="J13" s="67"/>
       <c r="K13" s="67"/>
-      <c r="L13" s="67"/>
+      <c r="L13" s="80"/>
       <c r="M13" s="67"/>
       <c r="N13" s="67"/>
       <c r="O13" s="70"/>
@@ -3431,7 +3458,7 @@
       <c r="Q13" s="68"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="82" t="s">
+      <c r="B14" s="85" t="s">
         <v>95</v>
       </c>
       <c r="C14" s="78"/>
@@ -3440,17 +3467,17 @@
       <c r="F14" s="65"/>
       <c r="G14" s="67"/>
       <c r="H14" s="68"/>
-      <c r="I14" s="69"/>
+      <c r="I14" s="81"/>
       <c r="J14" s="67"/>
       <c r="K14" s="67"/>
-      <c r="L14" s="67"/>
+      <c r="L14" s="80"/>
       <c r="M14" s="67"/>
       <c r="N14" s="67"/>
       <c r="O14" s="70"/>
       <c r="P14" s="70"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="82" t="s">
+      <c r="B15" s="85" t="s">
         <v>97</v>
       </c>
       <c r="C15" s="78"/>
@@ -3459,17 +3486,17 @@
       <c r="F15" s="65"/>
       <c r="G15" s="67"/>
       <c r="H15" s="68"/>
-      <c r="I15" s="69"/>
-      <c r="J15" s="67"/>
+      <c r="I15" s="81"/>
+      <c r="J15" s="80"/>
       <c r="K15" s="67"/>
-      <c r="L15" s="67"/>
-      <c r="M15" s="67"/>
+      <c r="L15" s="80"/>
+      <c r="M15" s="80"/>
       <c r="N15" s="67"/>
       <c r="O15" s="70"/>
       <c r="P15" s="70"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="82" t="s">
+      <c r="B16" s="85" t="s">
         <v>99</v>
       </c>
       <c r="C16" s="78"/>
@@ -3479,16 +3506,16 @@
       <c r="G16" s="67"/>
       <c r="H16" s="68"/>
       <c r="I16" s="69"/>
-      <c r="J16" s="67"/>
-      <c r="K16" s="67"/>
+      <c r="J16" s="80"/>
+      <c r="K16" s="80"/>
       <c r="L16" s="67"/>
-      <c r="M16" s="67"/>
-      <c r="N16" s="67"/>
+      <c r="M16" s="80"/>
+      <c r="N16" s="80"/>
       <c r="O16" s="70"/>
       <c r="P16" s="70"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="82" t="s">
+      <c r="B17" s="85" t="s">
         <v>101</v>
       </c>
       <c r="C17" s="78"/>
@@ -3498,273 +3525,285 @@
       <c r="G17" s="67"/>
       <c r="H17" s="68"/>
       <c r="I17" s="69"/>
-      <c r="J17" s="67"/>
+      <c r="J17" s="80"/>
       <c r="K17" s="67"/>
       <c r="L17" s="67"/>
-      <c r="M17" s="67"/>
-      <c r="N17" s="67"/>
+      <c r="M17" s="80"/>
+      <c r="N17" s="86"/>
       <c r="O17" s="70"/>
       <c r="P17" s="70"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="82" t="s">
+      <c r="B18" s="85" t="s">
         <v>103</v>
       </c>
-      <c r="C18" s="83"/>
-      <c r="D18" s="84"/>
-      <c r="E18" s="85"/>
-      <c r="F18" s="84"/>
-      <c r="G18" s="86"/>
-      <c r="H18" s="87"/>
-      <c r="I18" s="88"/>
-      <c r="J18" s="86"/>
-      <c r="K18" s="86"/>
-      <c r="L18" s="86"/>
-      <c r="M18" s="86"/>
-      <c r="N18" s="86"/>
-      <c r="O18" s="89"/>
-      <c r="P18" s="89"/>
+      <c r="C18" s="87"/>
+      <c r="D18" s="88"/>
+      <c r="E18" s="89"/>
+      <c r="F18" s="88"/>
+      <c r="G18" s="90"/>
+      <c r="H18" s="91"/>
+      <c r="I18" s="92"/>
+      <c r="J18" s="90"/>
+      <c r="K18" s="93"/>
+      <c r="L18" s="90"/>
+      <c r="M18" s="90"/>
+      <c r="N18" s="93"/>
+      <c r="O18" s="94"/>
+      <c r="P18" s="94"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="90" t="s">
+      <c r="B19" s="95" t="s">
         <v>121</v>
       </c>
-      <c r="C19" s="91" t="n">
+      <c r="C19" s="96" t="n">
         <v>4</v>
       </c>
-      <c r="D19" s="92" t="n">
+      <c r="D19" s="97" t="n">
         <v>9</v>
       </c>
-      <c r="E19" s="93" t="n">
+      <c r="E19" s="98" t="n">
         <v>9</v>
       </c>
-      <c r="F19" s="92" t="n">
+      <c r="F19" s="97" t="n">
         <v>12</v>
       </c>
-      <c r="G19" s="94" t="n">
+      <c r="G19" s="99" t="n">
         <v>12</v>
       </c>
-      <c r="H19" s="95"/>
-      <c r="I19" s="92" t="n">
+      <c r="H19" s="100"/>
+      <c r="I19" s="97" t="n">
         <v>13</v>
       </c>
-      <c r="J19" s="94" t="n">
+      <c r="J19" s="99" t="n">
         <v>13</v>
       </c>
-      <c r="K19" s="94" t="n">
+      <c r="K19" s="99" t="n">
         <v>13</v>
       </c>
-      <c r="L19" s="94" t="n">
+      <c r="L19" s="99" t="n">
         <v>13</v>
       </c>
-      <c r="M19" s="94" t="n">
+      <c r="M19" s="99" t="n">
         <v>13</v>
       </c>
-      <c r="N19" s="94" t="n">
+      <c r="N19" s="99" t="n">
         <v>13</v>
       </c>
-      <c r="O19" s="96"/>
-      <c r="P19" s="96"/>
-      <c r="Q19" s="95"/>
+      <c r="O19" s="101"/>
+      <c r="P19" s="101"/>
+      <c r="Q19" s="100"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="90" t="s">
+      <c r="B20" s="95" t="s">
         <v>122</v>
       </c>
-      <c r="C20" s="91" t="n">
+      <c r="C20" s="96" t="n">
         <v>2</v>
       </c>
-      <c r="D20" s="92" t="n">
+      <c r="D20" s="97" t="n">
         <v>7</v>
       </c>
-      <c r="E20" s="93" t="n">
+      <c r="E20" s="98" t="n">
         <v>7</v>
       </c>
-      <c r="F20" s="92" t="n">
+      <c r="F20" s="97" t="n">
         <v>9</v>
       </c>
-      <c r="G20" s="94" t="n">
+      <c r="G20" s="99" t="n">
         <v>7</v>
       </c>
-      <c r="H20" s="95"/>
-      <c r="I20" s="92"/>
-      <c r="J20" s="94"/>
-      <c r="K20" s="94"/>
-      <c r="L20" s="94"/>
-      <c r="M20" s="94"/>
-      <c r="N20" s="94"/>
-      <c r="O20" s="96"/>
-      <c r="P20" s="96"/>
-      <c r="Q20" s="95"/>
+      <c r="H20" s="100"/>
+      <c r="I20" s="97" t="n">
+        <v>9</v>
+      </c>
+      <c r="J20" s="99" t="n">
+        <v>9</v>
+      </c>
+      <c r="K20" s="99" t="n">
+        <v>9</v>
+      </c>
+      <c r="L20" s="99" t="n">
+        <v>7</v>
+      </c>
+      <c r="M20" s="99" t="n">
+        <v>7</v>
+      </c>
+      <c r="N20" s="99" t="n">
+        <v>7</v>
+      </c>
+      <c r="O20" s="101"/>
+      <c r="P20" s="101"/>
+      <c r="Q20" s="100"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="97" t="s">
+      <c r="B21" s="102" t="s">
         <v>123</v>
       </c>
-      <c r="C21" s="98" t="n">
+      <c r="C21" s="103" t="n">
         <v>1</v>
       </c>
-      <c r="D21" s="99" t="n">
+      <c r="D21" s="104" t="n">
         <v>1</v>
       </c>
-      <c r="E21" s="100" t="n">
+      <c r="E21" s="105" t="n">
         <v>1</v>
       </c>
-      <c r="F21" s="99" t="n">
+      <c r="F21" s="104" t="n">
         <v>1</v>
       </c>
-      <c r="G21" s="101" t="n">
+      <c r="G21" s="106" t="n">
         <v>1</v>
       </c>
-      <c r="H21" s="95"/>
-      <c r="I21" s="99" t="n">
+      <c r="H21" s="100"/>
+      <c r="I21" s="104" t="n">
         <v>1</v>
       </c>
-      <c r="J21" s="101" t="n">
+      <c r="J21" s="106" t="n">
         <v>1</v>
       </c>
-      <c r="K21" s="101" t="n">
+      <c r="K21" s="106" t="n">
         <v>1</v>
       </c>
-      <c r="L21" s="101" t="n">
+      <c r="L21" s="106" t="n">
         <v>1</v>
       </c>
-      <c r="M21" s="101" t="n">
+      <c r="M21" s="106" t="n">
         <v>1</v>
       </c>
-      <c r="N21" s="101" t="n">
+      <c r="N21" s="106" t="n">
         <v>1</v>
       </c>
-      <c r="O21" s="96"/>
-      <c r="P21" s="96"/>
-      <c r="Q21" s="95"/>
+      <c r="O21" s="101"/>
+      <c r="P21" s="101"/>
+      <c r="Q21" s="100"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="102" t="s">
+      <c r="B22" s="107" t="s">
         <v>124</v>
       </c>
-      <c r="C22" s="103" t="n">
+      <c r="C22" s="108" t="n">
         <f aca="false">C19-C20</f>
         <v>2</v>
       </c>
-      <c r="D22" s="104" t="n">
+      <c r="D22" s="109" t="n">
         <f aca="false">D19-D20</f>
         <v>2</v>
       </c>
-      <c r="E22" s="105" t="n">
+      <c r="E22" s="110" t="n">
         <f aca="false">E19-E20</f>
         <v>2</v>
       </c>
-      <c r="F22" s="104" t="n">
+      <c r="F22" s="109" t="n">
         <f aca="false">F19-F20</f>
         <v>3</v>
       </c>
-      <c r="G22" s="106" t="n">
+      <c r="G22" s="111" t="n">
         <f aca="false">G19-G20</f>
         <v>5</v>
       </c>
-      <c r="H22" s="95" t="n">
+      <c r="H22" s="100" t="n">
         <f aca="false">H19-H20</f>
         <v>0</v>
       </c>
-      <c r="I22" s="104" t="n">
+      <c r="I22" s="109" t="n">
         <f aca="false">I19-I20</f>
-        <v>13</v>
-      </c>
-      <c r="J22" s="106" t="n">
+        <v>4</v>
+      </c>
+      <c r="J22" s="111" t="n">
         <f aca="false">J19-J20</f>
-        <v>13</v>
-      </c>
-      <c r="K22" s="106" t="n">
+        <v>4</v>
+      </c>
+      <c r="K22" s="111" t="n">
         <f aca="false">K19-K20</f>
-        <v>13</v>
-      </c>
-      <c r="L22" s="106" t="n">
+        <v>4</v>
+      </c>
+      <c r="L22" s="111" t="n">
         <f aca="false">L19-L20</f>
-        <v>13</v>
-      </c>
-      <c r="M22" s="106" t="n">
+        <v>6</v>
+      </c>
+      <c r="M22" s="111" t="n">
         <f aca="false">M19-M20</f>
-        <v>13</v>
-      </c>
-      <c r="N22" s="106" t="n">
+        <v>6</v>
+      </c>
+      <c r="N22" s="111" t="n">
         <f aca="false">N19-N20</f>
-        <v>13</v>
-      </c>
-      <c r="O22" s="96" t="n">
+        <v>6</v>
+      </c>
+      <c r="O22" s="101" t="n">
         <f aca="false">O19-O20</f>
         <v>0</v>
       </c>
-      <c r="P22" s="96" t="n">
+      <c r="P22" s="101" t="n">
         <f aca="false">P19-P20</f>
         <v>0</v>
       </c>
-      <c r="Q22" s="95" t="n">
+      <c r="Q22" s="100" t="n">
         <f aca="false">Q19-Q20</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="107" t="s">
+      <c r="B23" s="112" t="s">
         <v>125</v>
       </c>
-      <c r="C23" s="108" t="n">
+      <c r="C23" s="113" t="n">
         <f aca="false">C22+C21</f>
         <v>3</v>
       </c>
-      <c r="D23" s="109" t="n">
+      <c r="D23" s="114" t="n">
         <f aca="false">D22+D21</f>
         <v>3</v>
       </c>
-      <c r="E23" s="110" t="n">
+      <c r="E23" s="115" t="n">
         <f aca="false">E22+E21</f>
         <v>3</v>
       </c>
-      <c r="F23" s="109" t="n">
+      <c r="F23" s="114" t="n">
         <f aca="false">F22+F21</f>
         <v>4</v>
       </c>
-      <c r="G23" s="111" t="n">
+      <c r="G23" s="116" t="n">
         <f aca="false">G22+G21</f>
         <v>6</v>
       </c>
-      <c r="H23" s="95" t="n">
+      <c r="H23" s="100" t="n">
         <f aca="false">H22+H21</f>
         <v>0</v>
       </c>
-      <c r="I23" s="109" t="n">
+      <c r="I23" s="114" t="n">
         <f aca="false">I22+I21</f>
-        <v>14</v>
-      </c>
-      <c r="J23" s="111" t="n">
+        <v>5</v>
+      </c>
+      <c r="J23" s="116" t="n">
         <f aca="false">J22+J21</f>
-        <v>14</v>
-      </c>
-      <c r="K23" s="111" t="n">
+        <v>5</v>
+      </c>
+      <c r="K23" s="116" t="n">
         <f aca="false">K22+K21</f>
-        <v>14</v>
-      </c>
-      <c r="L23" s="111" t="n">
+        <v>5</v>
+      </c>
+      <c r="L23" s="116" t="n">
         <f aca="false">L22+L21</f>
-        <v>14</v>
-      </c>
-      <c r="M23" s="111" t="n">
+        <v>7</v>
+      </c>
+      <c r="M23" s="116" t="n">
         <f aca="false">M22+M21</f>
-        <v>14</v>
-      </c>
-      <c r="N23" s="111" t="n">
+        <v>7</v>
+      </c>
+      <c r="N23" s="116" t="n">
         <f aca="false">N22+N21</f>
-        <v>14</v>
-      </c>
-      <c r="O23" s="96" t="n">
+        <v>7</v>
+      </c>
+      <c r="O23" s="101" t="n">
         <f aca="false">O22+O21</f>
         <v>0</v>
       </c>
-      <c r="P23" s="96" t="n">
+      <c r="P23" s="101" t="n">
         <f aca="false">P22+P21</f>
         <v>0</v>
       </c>
-      <c r="Q23" s="95" t="n">
+      <c r="Q23" s="100" t="n">
         <f aca="false">Q22+Q21</f>
         <v>0</v>
       </c>
@@ -3932,10 +3971,10 @@
       <c r="H31" s="68"/>
       <c r="I31" s="69"/>
       <c r="J31" s="67"/>
-      <c r="K31" s="67"/>
+      <c r="K31" s="80"/>
       <c r="L31" s="67"/>
       <c r="M31" s="67"/>
-      <c r="N31" s="67"/>
+      <c r="N31" s="80"/>
       <c r="O31" s="70"/>
       <c r="P31" s="70"/>
       <c r="Q31" s="68"/>
@@ -3950,12 +3989,12 @@
       <c r="F32" s="71"/>
       <c r="G32" s="80"/>
       <c r="H32" s="68"/>
-      <c r="I32" s="69"/>
-      <c r="J32" s="67"/>
-      <c r="K32" s="67"/>
-      <c r="L32" s="67"/>
-      <c r="M32" s="67"/>
-      <c r="N32" s="67"/>
+      <c r="I32" s="81"/>
+      <c r="J32" s="80"/>
+      <c r="K32" s="80"/>
+      <c r="L32" s="80"/>
+      <c r="M32" s="80"/>
+      <c r="N32" s="80"/>
       <c r="O32" s="70"/>
       <c r="P32" s="70"/>
       <c r="Q32" s="68"/>
@@ -3984,18 +4023,18 @@
       <c r="B34" s="77" t="s">
         <v>83</v>
       </c>
-      <c r="C34" s="112"/>
-      <c r="D34" s="113"/>
-      <c r="E34" s="114"/>
-      <c r="F34" s="113"/>
-      <c r="G34" s="81"/>
+      <c r="C34" s="117"/>
+      <c r="D34" s="118"/>
+      <c r="E34" s="119"/>
+      <c r="F34" s="118"/>
+      <c r="G34" s="82"/>
       <c r="H34" s="68"/>
-      <c r="I34" s="115"/>
-      <c r="J34" s="81"/>
-      <c r="K34" s="81"/>
-      <c r="L34" s="81"/>
-      <c r="M34" s="81"/>
-      <c r="N34" s="81"/>
+      <c r="I34" s="120"/>
+      <c r="J34" s="82"/>
+      <c r="K34" s="82"/>
+      <c r="L34" s="82"/>
+      <c r="M34" s="82"/>
+      <c r="N34" s="82"/>
       <c r="O34" s="70"/>
       <c r="P34" s="70"/>
       <c r="Q34" s="68"/>
@@ -4004,18 +4043,18 @@
       <c r="B35" s="77" t="s">
         <v>86</v>
       </c>
-      <c r="C35" s="112"/>
-      <c r="D35" s="113"/>
-      <c r="E35" s="114"/>
-      <c r="F35" s="113"/>
-      <c r="G35" s="81"/>
+      <c r="C35" s="117"/>
+      <c r="D35" s="118"/>
+      <c r="E35" s="119"/>
+      <c r="F35" s="118"/>
+      <c r="G35" s="82"/>
       <c r="H35" s="68"/>
-      <c r="I35" s="115"/>
-      <c r="J35" s="81"/>
-      <c r="K35" s="81"/>
-      <c r="L35" s="81"/>
-      <c r="M35" s="81"/>
-      <c r="N35" s="81"/>
+      <c r="I35" s="120"/>
+      <c r="J35" s="82"/>
+      <c r="K35" s="82"/>
+      <c r="L35" s="82"/>
+      <c r="M35" s="82"/>
+      <c r="N35" s="82"/>
       <c r="O35" s="70"/>
       <c r="P35" s="70"/>
       <c r="Q35" s="68"/>
@@ -4030,10 +4069,10 @@
       <c r="F36" s="65"/>
       <c r="G36" s="67"/>
       <c r="H36" s="68"/>
-      <c r="I36" s="69"/>
+      <c r="I36" s="81"/>
       <c r="J36" s="67"/>
       <c r="K36" s="67"/>
-      <c r="L36" s="67"/>
+      <c r="L36" s="80"/>
       <c r="M36" s="67"/>
       <c r="N36" s="67"/>
       <c r="O36" s="70"/>
@@ -4041,7 +4080,7 @@
       <c r="Q36" s="68"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="82" t="s">
+      <c r="B37" s="85" t="s">
         <v>95</v>
       </c>
       <c r="C37" s="78"/>
@@ -4050,17 +4089,17 @@
       <c r="F37" s="65"/>
       <c r="G37" s="67"/>
       <c r="H37" s="68"/>
-      <c r="I37" s="69"/>
+      <c r="I37" s="81"/>
       <c r="J37" s="67"/>
       <c r="K37" s="67"/>
-      <c r="L37" s="67"/>
+      <c r="L37" s="80"/>
       <c r="M37" s="67"/>
       <c r="N37" s="67"/>
       <c r="O37" s="70"/>
       <c r="P37" s="70"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="82" t="s">
+      <c r="B38" s="85" t="s">
         <v>97</v>
       </c>
       <c r="C38" s="78"/>
@@ -4069,17 +4108,17 @@
       <c r="F38" s="65"/>
       <c r="G38" s="67"/>
       <c r="H38" s="68"/>
-      <c r="I38" s="69"/>
-      <c r="J38" s="67"/>
+      <c r="I38" s="81"/>
+      <c r="J38" s="80"/>
       <c r="K38" s="67"/>
-      <c r="L38" s="67"/>
-      <c r="M38" s="67"/>
+      <c r="L38" s="80"/>
+      <c r="M38" s="80"/>
       <c r="N38" s="67"/>
       <c r="O38" s="70"/>
       <c r="P38" s="70"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="82" t="s">
+      <c r="B39" s="85" t="s">
         <v>99</v>
       </c>
       <c r="C39" s="78"/>
@@ -4089,16 +4128,16 @@
       <c r="G39" s="67"/>
       <c r="H39" s="68"/>
       <c r="I39" s="69"/>
-      <c r="J39" s="67"/>
-      <c r="K39" s="67"/>
-      <c r="L39" s="67"/>
-      <c r="M39" s="67"/>
-      <c r="N39" s="67"/>
+      <c r="J39" s="80"/>
+      <c r="K39" s="80"/>
+      <c r="L39" s="86"/>
+      <c r="M39" s="80"/>
+      <c r="N39" s="80"/>
       <c r="O39" s="70"/>
       <c r="P39" s="70"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="82" t="s">
+      <c r="B40" s="85" t="s">
         <v>101</v>
       </c>
       <c r="C40" s="78"/>
@@ -4108,273 +4147,285 @@
       <c r="G40" s="67"/>
       <c r="H40" s="68"/>
       <c r="I40" s="69"/>
-      <c r="J40" s="67"/>
+      <c r="J40" s="80"/>
       <c r="K40" s="67"/>
       <c r="L40" s="67"/>
-      <c r="M40" s="67"/>
+      <c r="M40" s="80"/>
       <c r="N40" s="67"/>
       <c r="O40" s="70"/>
       <c r="P40" s="70"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="82" t="s">
+      <c r="B41" s="85" t="s">
         <v>103</v>
       </c>
-      <c r="C41" s="83"/>
-      <c r="D41" s="84"/>
-      <c r="E41" s="85"/>
-      <c r="F41" s="84"/>
-      <c r="G41" s="86"/>
-      <c r="H41" s="87"/>
-      <c r="I41" s="88"/>
-      <c r="J41" s="86"/>
-      <c r="K41" s="86"/>
-      <c r="L41" s="86"/>
-      <c r="M41" s="86"/>
-      <c r="N41" s="86"/>
-      <c r="O41" s="89"/>
-      <c r="P41" s="89"/>
+      <c r="C41" s="87"/>
+      <c r="D41" s="88"/>
+      <c r="E41" s="89"/>
+      <c r="F41" s="88"/>
+      <c r="G41" s="90"/>
+      <c r="H41" s="91"/>
+      <c r="I41" s="92"/>
+      <c r="J41" s="90"/>
+      <c r="K41" s="93"/>
+      <c r="L41" s="90"/>
+      <c r="M41" s="90"/>
+      <c r="N41" s="93"/>
+      <c r="O41" s="94"/>
+      <c r="P41" s="94"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="90" t="s">
+      <c r="B42" s="95" t="s">
         <v>121</v>
       </c>
-      <c r="C42" s="91" t="n">
+      <c r="C42" s="96" t="n">
         <v>4</v>
       </c>
-      <c r="D42" s="92" t="n">
+      <c r="D42" s="97" t="n">
         <v>9</v>
       </c>
-      <c r="E42" s="93" t="n">
+      <c r="E42" s="98" t="n">
         <v>9</v>
       </c>
-      <c r="F42" s="92" t="n">
+      <c r="F42" s="97" t="n">
         <v>12</v>
       </c>
-      <c r="G42" s="94" t="n">
+      <c r="G42" s="99" t="n">
         <v>12</v>
       </c>
-      <c r="H42" s="95"/>
-      <c r="I42" s="92" t="n">
+      <c r="H42" s="100"/>
+      <c r="I42" s="97" t="n">
         <v>13</v>
       </c>
-      <c r="J42" s="94" t="n">
+      <c r="J42" s="99" t="n">
         <v>13</v>
       </c>
-      <c r="K42" s="94" t="n">
+      <c r="K42" s="99" t="n">
         <v>13</v>
       </c>
-      <c r="L42" s="94" t="n">
+      <c r="L42" s="99" t="n">
         <v>13</v>
       </c>
-      <c r="M42" s="94" t="n">
+      <c r="M42" s="99" t="n">
         <v>13</v>
       </c>
-      <c r="N42" s="94" t="n">
+      <c r="N42" s="99" t="n">
         <v>13</v>
       </c>
-      <c r="O42" s="96"/>
-      <c r="P42" s="96"/>
-      <c r="Q42" s="95"/>
-    </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="90" t="s">
+      <c r="O42" s="101"/>
+      <c r="P42" s="101"/>
+      <c r="Q42" s="100"/>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="95" t="s">
         <v>122</v>
       </c>
-      <c r="C43" s="91" t="n">
+      <c r="C43" s="96" t="n">
         <v>2</v>
       </c>
-      <c r="D43" s="92" t="n">
+      <c r="D43" s="97" t="n">
         <v>7</v>
       </c>
-      <c r="E43" s="93" t="n">
+      <c r="E43" s="98" t="n">
         <v>7</v>
       </c>
-      <c r="F43" s="92" t="n">
+      <c r="F43" s="97" t="n">
         <v>9</v>
       </c>
-      <c r="G43" s="94" t="n">
+      <c r="G43" s="99" t="n">
         <v>7</v>
       </c>
-      <c r="H43" s="95"/>
-      <c r="I43" s="92"/>
-      <c r="J43" s="94"/>
-      <c r="K43" s="94"/>
-      <c r="L43" s="94"/>
-      <c r="M43" s="94"/>
-      <c r="N43" s="94"/>
-      <c r="O43" s="96"/>
-      <c r="P43" s="96"/>
-      <c r="Q43" s="95"/>
+      <c r="H43" s="100"/>
+      <c r="I43" s="97" t="n">
+        <v>9</v>
+      </c>
+      <c r="J43" s="99" t="n">
+        <v>9</v>
+      </c>
+      <c r="K43" s="99" t="n">
+        <v>9</v>
+      </c>
+      <c r="L43" s="99" t="n">
+        <v>7</v>
+      </c>
+      <c r="M43" s="99" t="n">
+        <v>7</v>
+      </c>
+      <c r="N43" s="99" t="n">
+        <v>7</v>
+      </c>
+      <c r="O43" s="101"/>
+      <c r="P43" s="101"/>
+      <c r="Q43" s="100"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="97" t="s">
+      <c r="B44" s="102" t="s">
         <v>123</v>
       </c>
-      <c r="C44" s="98" t="n">
+      <c r="C44" s="103" t="n">
         <v>3</v>
       </c>
-      <c r="D44" s="99" t="n">
+      <c r="D44" s="104" t="n">
         <v>3</v>
       </c>
-      <c r="E44" s="100" t="n">
+      <c r="E44" s="105" t="n">
         <v>3</v>
       </c>
-      <c r="F44" s="99" t="n">
+      <c r="F44" s="104" t="n">
         <v>3</v>
       </c>
-      <c r="G44" s="101" t="n">
+      <c r="G44" s="106" t="n">
         <v>3</v>
       </c>
-      <c r="H44" s="95"/>
-      <c r="I44" s="99" t="n">
+      <c r="H44" s="100"/>
+      <c r="I44" s="104" t="n">
         <v>3</v>
       </c>
-      <c r="J44" s="101" t="n">
+      <c r="J44" s="106" t="n">
         <v>3</v>
       </c>
-      <c r="K44" s="101" t="n">
+      <c r="K44" s="106" t="n">
         <v>3</v>
       </c>
-      <c r="L44" s="101" t="n">
+      <c r="L44" s="106" t="n">
         <v>3</v>
       </c>
-      <c r="M44" s="101" t="n">
+      <c r="M44" s="106" t="n">
         <v>3</v>
       </c>
-      <c r="N44" s="101" t="n">
+      <c r="N44" s="106" t="n">
         <v>3</v>
       </c>
-      <c r="O44" s="96"/>
-      <c r="P44" s="96"/>
-      <c r="Q44" s="95"/>
+      <c r="O44" s="101"/>
+      <c r="P44" s="101"/>
+      <c r="Q44" s="100"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="102" t="s">
+      <c r="B45" s="107" t="s">
         <v>124</v>
       </c>
-      <c r="C45" s="103" t="n">
+      <c r="C45" s="108" t="n">
         <f aca="false">C42-C43</f>
         <v>2</v>
       </c>
-      <c r="D45" s="104" t="n">
+      <c r="D45" s="109" t="n">
         <f aca="false">D42-D43</f>
         <v>2</v>
       </c>
-      <c r="E45" s="105" t="n">
+      <c r="E45" s="110" t="n">
         <f aca="false">E42-E43</f>
         <v>2</v>
       </c>
-      <c r="F45" s="104" t="n">
+      <c r="F45" s="109" t="n">
         <f aca="false">F42-F43</f>
         <v>3</v>
       </c>
-      <c r="G45" s="106" t="n">
+      <c r="G45" s="111" t="n">
         <f aca="false">G42-G43</f>
         <v>5</v>
       </c>
-      <c r="H45" s="95" t="n">
+      <c r="H45" s="100" t="n">
         <f aca="false">H42-H43</f>
         <v>0</v>
       </c>
-      <c r="I45" s="104" t="n">
+      <c r="I45" s="109" t="n">
         <f aca="false">I42-I43</f>
-        <v>13</v>
-      </c>
-      <c r="J45" s="106" t="n">
+        <v>4</v>
+      </c>
+      <c r="J45" s="111" t="n">
         <f aca="false">J42-J43</f>
-        <v>13</v>
-      </c>
-      <c r="K45" s="106" t="n">
+        <v>4</v>
+      </c>
+      <c r="K45" s="111" t="n">
         <f aca="false">K42-K43</f>
-        <v>13</v>
-      </c>
-      <c r="L45" s="106" t="n">
+        <v>4</v>
+      </c>
+      <c r="L45" s="111" t="n">
         <f aca="false">L42-L43</f>
-        <v>13</v>
-      </c>
-      <c r="M45" s="106" t="n">
+        <v>6</v>
+      </c>
+      <c r="M45" s="111" t="n">
         <f aca="false">M42-M43</f>
-        <v>13</v>
-      </c>
-      <c r="N45" s="106" t="n">
+        <v>6</v>
+      </c>
+      <c r="N45" s="111" t="n">
         <f aca="false">N42-N43</f>
-        <v>13</v>
-      </c>
-      <c r="O45" s="96" t="n">
+        <v>6</v>
+      </c>
+      <c r="O45" s="101" t="n">
         <f aca="false">O42-O43</f>
         <v>0</v>
       </c>
-      <c r="P45" s="96" t="n">
+      <c r="P45" s="101" t="n">
         <f aca="false">P42-P43</f>
         <v>0</v>
       </c>
-      <c r="Q45" s="95" t="n">
+      <c r="Q45" s="100" t="n">
         <f aca="false">Q42-Q43</f>
         <v>0</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="107" t="s">
+      <c r="B46" s="112" t="s">
         <v>125</v>
       </c>
-      <c r="C46" s="108" t="n">
+      <c r="C46" s="113" t="n">
         <f aca="false">C45+C44</f>
         <v>5</v>
       </c>
-      <c r="D46" s="109" t="n">
+      <c r="D46" s="114" t="n">
         <f aca="false">D45+D44</f>
         <v>5</v>
       </c>
-      <c r="E46" s="110" t="n">
+      <c r="E46" s="115" t="n">
         <f aca="false">E45+E44</f>
         <v>5</v>
       </c>
-      <c r="F46" s="109" t="n">
+      <c r="F46" s="114" t="n">
         <f aca="false">F45+F44</f>
         <v>6</v>
       </c>
-      <c r="G46" s="111" t="n">
+      <c r="G46" s="116" t="n">
         <f aca="false">G45+G44</f>
         <v>8</v>
       </c>
-      <c r="H46" s="95" t="n">
+      <c r="H46" s="100" t="n">
         <f aca="false">H45+H44</f>
         <v>0</v>
       </c>
-      <c r="I46" s="109" t="n">
+      <c r="I46" s="114" t="n">
         <f aca="false">I45+I44</f>
-        <v>16</v>
-      </c>
-      <c r="J46" s="111" t="n">
+        <v>7</v>
+      </c>
+      <c r="J46" s="116" t="n">
         <f aca="false">J45+J44</f>
-        <v>16</v>
-      </c>
-      <c r="K46" s="111" t="n">
+        <v>7</v>
+      </c>
+      <c r="K46" s="116" t="n">
         <f aca="false">K45+K44</f>
-        <v>16</v>
-      </c>
-      <c r="L46" s="111" t="n">
+        <v>7</v>
+      </c>
+      <c r="L46" s="116" t="n">
         <f aca="false">L45+L44</f>
-        <v>16</v>
-      </c>
-      <c r="M46" s="111" t="n">
+        <v>9</v>
+      </c>
+      <c r="M46" s="116" t="n">
         <f aca="false">M45+M44</f>
-        <v>16</v>
-      </c>
-      <c r="N46" s="111" t="n">
+        <v>9</v>
+      </c>
+      <c r="N46" s="116" t="n">
         <f aca="false">N45+N44</f>
-        <v>16</v>
-      </c>
-      <c r="O46" s="96" t="n">
+        <v>9</v>
+      </c>
+      <c r="O46" s="101" t="n">
         <f aca="false">O45+O44</f>
         <v>0</v>
       </c>
-      <c r="P46" s="96" t="n">
+      <c r="P46" s="101" t="n">
         <f aca="false">P45+P44</f>
         <v>0</v>
       </c>
-      <c r="Q46" s="95" t="n">
+      <c r="Q46" s="100" t="n">
         <f aca="false">Q45+Q44</f>
         <v>0</v>
       </c>

</xml_diff>